<commit_message>
csv upload und schreiben was gesehen wurde
</commit_message>
<xml_diff>
--- a/All_missions.xlsx
+++ b/All_missions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sabin\Desktop\FHNW\LERNMATERIALIEN\4 SEM\KOMP\cda2 Robo Challenge\robot_challenge_fs25\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\silas\PycharmProjects\Robo_challenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C7EE32F-8F93-4B3B-BB00-5F70750F9DA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E568DB6B-4F98-4D87-9D4D-39E41642BE68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="84">
   <si>
     <t>Main Tasks</t>
   </si>
@@ -311,6 +311,107 @@
   <si>
     <t>find_face</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Speichern Sie relevante Informationen während der Fahrt in einer CSV-Datei (comma-separated-values) in geeigneten Datenstrukturen. 
+•	</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Erfassen Sie Zeitstempel für den Beginn der Fahrt, die Einfahrt in die Finisher-Box und für et-waige Wendemanöver.
+•	Berechnen Sie die Gesamtdauer Ihrer Fahrt von der Startposition bis zur Zielbox in Minuten und Sekunden (z. B. 5 Minuten 30 Sekunden). 
+•	Führen Sie Aufzeichnungen für jedes auf der Straße erkannte Objekt, einschließlich des Zeit-stempels der Erkennung. Zählen Sie auch die Gesamtzahl der erkannten Objekte.
+•	Führen Sie für jedes erkannte Gesicht einen Datensatz, der mindestens den Zeitstempel der Erkennung enthält. Verfolgen Sie auch die Gesamtzahl der erkannten Gesichter. Es gibt immer nur ein Gesicht pro Standort.</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+•	</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Führen Sie einen Datensatz für jedes Objekt und jeden QR-Code, den Sie während der Fahrt erkannt haben. Speichern Sie mindestens die folgenden Informationen pro Objekt: Zeitstempel, wann ein QR-Code gelesen wurde, Informationen, die Sie gelesen/gelesen haben, Aktion, die Sie durchgeführt haben. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+•	</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Erfassen Sie, wann Sie einen (rechteckigen) Kreisverkehr betreten und verlassen haben.</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+•	</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Der QR-Code für den Spinntrick wurde geparst und in der CSV-Datei mit einem Zeitstempel protokolliert.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+•	Speichern Sie am Ende des Laufs die Kartendaten in einer separaten CSV-Datei.
+•	Speichern Sie andere Informationen, die Sie für wichtig halten.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -319,7 +420,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -363,6 +464,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -953,6 +1070,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -997,45 +1153,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1379,8 +1496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:Y62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="M38" sqref="M38"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1399,17 +1516,17 @@
   <sheetData>
     <row r="1" spans="2:25" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:25" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="60" t="s">
+      <c r="B2" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="61"/>
-      <c r="I2" s="61"/>
-      <c r="J2" s="62"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="48"/>
       <c r="M2" s="33" t="s">
         <v>27</v>
       </c>
@@ -1417,49 +1534,49 @@
         <v>28</v>
       </c>
       <c r="O2" s="34"/>
-      <c r="P2" s="57" t="s">
+      <c r="P2" s="70" t="s">
         <v>46</v>
       </c>
-      <c r="Q2" s="57"/>
-      <c r="R2" s="57"/>
-      <c r="S2" s="57"/>
-      <c r="T2" s="57"/>
-      <c r="U2" s="57"/>
-      <c r="V2" s="57"/>
-      <c r="W2" s="58"/>
+      <c r="Q2" s="70"/>
+      <c r="R2" s="70"/>
+      <c r="S2" s="70"/>
+      <c r="T2" s="70"/>
+      <c r="U2" s="70"/>
+      <c r="V2" s="70"/>
+      <c r="W2" s="71"/>
     </row>
     <row r="3" spans="2:25" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="63" t="s">
+      <c r="B3" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="65" t="s">
+      <c r="C3" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="65" t="s">
+      <c r="D3" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="65" t="s">
+      <c r="E3" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="65" t="s">
+      <c r="F3" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="67" t="s">
+      <c r="G3" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="69" t="s">
+      <c r="H3" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="70"/>
-      <c r="J3" s="71"/>
+      <c r="I3" s="56"/>
+      <c r="J3" s="57"/>
     </row>
     <row r="4" spans="2:25" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="64"/>
-      <c r="C4" s="66"/>
-      <c r="D4" s="66"/>
-      <c r="E4" s="66"/>
-      <c r="F4" s="66"/>
-      <c r="G4" s="68"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="54"/>
       <c r="H4" s="14" t="s">
         <v>14</v>
       </c>
@@ -1469,19 +1586,19 @@
       <c r="J4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="48" t="s">
-        <v>50</v>
-      </c>
-      <c r="N4" s="49"/>
-      <c r="O4" s="49"/>
-      <c r="P4" s="49"/>
-      <c r="Q4" s="49"/>
-      <c r="R4" s="49"/>
-      <c r="S4" s="49"/>
-      <c r="T4" s="49"/>
-      <c r="U4" s="49"/>
-      <c r="V4" s="49"/>
-      <c r="W4" s="50"/>
+      <c r="M4" s="61" t="s">
+        <v>83</v>
+      </c>
+      <c r="N4" s="62"/>
+      <c r="O4" s="62"/>
+      <c r="P4" s="62"/>
+      <c r="Q4" s="62"/>
+      <c r="R4" s="62"/>
+      <c r="S4" s="62"/>
+      <c r="T4" s="62"/>
+      <c r="U4" s="62"/>
+      <c r="V4" s="62"/>
+      <c r="W4" s="63"/>
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
     </row>
@@ -1495,19 +1612,19 @@
       <c r="H5" s="15"/>
       <c r="I5" s="9"/>
       <c r="J5" s="10"/>
-      <c r="M5" s="51"/>
-      <c r="N5" s="52"/>
-      <c r="O5" s="52"/>
-      <c r="P5" s="52"/>
-      <c r="Q5" s="52"/>
-      <c r="R5" s="52"/>
-      <c r="S5" s="52"/>
-      <c r="T5" s="52"/>
-      <c r="U5" s="52"/>
-      <c r="V5" s="52"/>
-      <c r="W5" s="53"/>
+      <c r="M5" s="64"/>
+      <c r="N5" s="65"/>
+      <c r="O5" s="65"/>
+      <c r="P5" s="65"/>
+      <c r="Q5" s="65"/>
+      <c r="R5" s="65"/>
+      <c r="S5" s="65"/>
+      <c r="T5" s="65"/>
+      <c r="U5" s="65"/>
+      <c r="V5" s="65"/>
+      <c r="W5" s="66"/>
       <c r="X5" s="1"/>
-      <c r="Y5" s="1"/>
+      <c r="Y5" s="35"/>
     </row>
     <row r="6" spans="2:25" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="37" t="s">
@@ -1529,17 +1646,17 @@
       </c>
       <c r="I6" s="42"/>
       <c r="J6" s="43"/>
-      <c r="M6" s="51"/>
-      <c r="N6" s="52"/>
-      <c r="O6" s="52"/>
-      <c r="P6" s="52"/>
-      <c r="Q6" s="52"/>
-      <c r="R6" s="52"/>
-      <c r="S6" s="52"/>
-      <c r="T6" s="52"/>
-      <c r="U6" s="52"/>
-      <c r="V6" s="52"/>
-      <c r="W6" s="53"/>
+      <c r="M6" s="64"/>
+      <c r="N6" s="65"/>
+      <c r="O6" s="65"/>
+      <c r="P6" s="65"/>
+      <c r="Q6" s="65"/>
+      <c r="R6" s="65"/>
+      <c r="S6" s="65"/>
+      <c r="T6" s="65"/>
+      <c r="U6" s="65"/>
+      <c r="V6" s="65"/>
+      <c r="W6" s="66"/>
       <c r="X6" s="1"/>
       <c r="Y6" s="1"/>
     </row>
@@ -1565,17 +1682,17 @@
         <v>1</v>
       </c>
       <c r="J7" s="43"/>
-      <c r="M7" s="51"/>
-      <c r="N7" s="52"/>
-      <c r="O7" s="52"/>
-      <c r="P7" s="52"/>
-      <c r="Q7" s="52"/>
-      <c r="R7" s="52"/>
-      <c r="S7" s="52"/>
-      <c r="T7" s="52"/>
-      <c r="U7" s="52"/>
-      <c r="V7" s="52"/>
-      <c r="W7" s="53"/>
+      <c r="M7" s="64"/>
+      <c r="N7" s="65"/>
+      <c r="O7" s="65"/>
+      <c r="P7" s="65"/>
+      <c r="Q7" s="65"/>
+      <c r="R7" s="65"/>
+      <c r="S7" s="65"/>
+      <c r="T7" s="65"/>
+      <c r="U7" s="65"/>
+      <c r="V7" s="65"/>
+      <c r="W7" s="66"/>
       <c r="X7" s="1"/>
       <c r="Y7" s="1"/>
     </row>
@@ -1593,7 +1710,7 @@
       <c r="F8" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="G8" s="72" t="s">
+      <c r="G8" s="45" t="s">
         <v>81</v>
       </c>
       <c r="H8" s="41"/>
@@ -1601,17 +1718,17 @@
         <v>1</v>
       </c>
       <c r="J8" s="43"/>
-      <c r="M8" s="51"/>
-      <c r="N8" s="52"/>
-      <c r="O8" s="52"/>
-      <c r="P8" s="52"/>
-      <c r="Q8" s="52"/>
-      <c r="R8" s="52"/>
-      <c r="S8" s="52"/>
-      <c r="T8" s="52"/>
-      <c r="U8" s="52"/>
-      <c r="V8" s="52"/>
-      <c r="W8" s="53"/>
+      <c r="M8" s="64"/>
+      <c r="N8" s="65"/>
+      <c r="O8" s="65"/>
+      <c r="P8" s="65"/>
+      <c r="Q8" s="65"/>
+      <c r="R8" s="65"/>
+      <c r="S8" s="65"/>
+      <c r="T8" s="65"/>
+      <c r="U8" s="65"/>
+      <c r="V8" s="65"/>
+      <c r="W8" s="66"/>
       <c r="X8" s="1"/>
       <c r="Y8" s="1"/>
     </row>
@@ -1637,17 +1754,17 @@
       </c>
       <c r="I9" s="17"/>
       <c r="J9" s="18"/>
-      <c r="M9" s="51"/>
-      <c r="N9" s="52"/>
-      <c r="O9" s="52"/>
-      <c r="P9" s="52"/>
-      <c r="Q9" s="52"/>
-      <c r="R9" s="52"/>
-      <c r="S9" s="52"/>
-      <c r="T9" s="52"/>
-      <c r="U9" s="52"/>
-      <c r="V9" s="52"/>
-      <c r="W9" s="53"/>
+      <c r="M9" s="64"/>
+      <c r="N9" s="65"/>
+      <c r="O9" s="65"/>
+      <c r="P9" s="65"/>
+      <c r="Q9" s="65"/>
+      <c r="R9" s="65"/>
+      <c r="S9" s="65"/>
+      <c r="T9" s="65"/>
+      <c r="U9" s="65"/>
+      <c r="V9" s="65"/>
+      <c r="W9" s="66"/>
       <c r="X9" s="1"/>
       <c r="Y9" s="1"/>
     </row>
@@ -1671,17 +1788,17 @@
         <v>1</v>
       </c>
       <c r="J10" s="18"/>
-      <c r="M10" s="51"/>
-      <c r="N10" s="52"/>
-      <c r="O10" s="52"/>
-      <c r="P10" s="52"/>
-      <c r="Q10" s="52"/>
-      <c r="R10" s="52"/>
-      <c r="S10" s="52"/>
-      <c r="T10" s="52"/>
-      <c r="U10" s="52"/>
-      <c r="V10" s="52"/>
-      <c r="W10" s="53"/>
+      <c r="M10" s="64"/>
+      <c r="N10" s="65"/>
+      <c r="O10" s="65"/>
+      <c r="P10" s="65"/>
+      <c r="Q10" s="65"/>
+      <c r="R10" s="65"/>
+      <c r="S10" s="65"/>
+      <c r="T10" s="65"/>
+      <c r="U10" s="65"/>
+      <c r="V10" s="65"/>
+      <c r="W10" s="66"/>
       <c r="X10" s="1"/>
       <c r="Y10" s="1"/>
     </row>
@@ -1705,17 +1822,17 @@
       <c r="J11" s="18">
         <v>1</v>
       </c>
-      <c r="M11" s="51"/>
-      <c r="N11" s="52"/>
-      <c r="O11" s="52"/>
-      <c r="P11" s="52"/>
-      <c r="Q11" s="52"/>
-      <c r="R11" s="52"/>
-      <c r="S11" s="52"/>
-      <c r="T11" s="52"/>
-      <c r="U11" s="52"/>
-      <c r="V11" s="52"/>
-      <c r="W11" s="53"/>
+      <c r="M11" s="64"/>
+      <c r="N11" s="65"/>
+      <c r="O11" s="65"/>
+      <c r="P11" s="65"/>
+      <c r="Q11" s="65"/>
+      <c r="R11" s="65"/>
+      <c r="S11" s="65"/>
+      <c r="T11" s="65"/>
+      <c r="U11" s="65"/>
+      <c r="V11" s="65"/>
+      <c r="W11" s="66"/>
       <c r="X11" s="1"/>
       <c r="Y11" s="1"/>
     </row>
@@ -1739,17 +1856,17 @@
         <v>1</v>
       </c>
       <c r="J12" s="18"/>
-      <c r="M12" s="51"/>
-      <c r="N12" s="52"/>
-      <c r="O12" s="52"/>
-      <c r="P12" s="52"/>
-      <c r="Q12" s="52"/>
-      <c r="R12" s="52"/>
-      <c r="S12" s="52"/>
-      <c r="T12" s="52"/>
-      <c r="U12" s="52"/>
-      <c r="V12" s="52"/>
-      <c r="W12" s="53"/>
+      <c r="M12" s="64"/>
+      <c r="N12" s="65"/>
+      <c r="O12" s="65"/>
+      <c r="P12" s="65"/>
+      <c r="Q12" s="65"/>
+      <c r="R12" s="65"/>
+      <c r="S12" s="65"/>
+      <c r="T12" s="65"/>
+      <c r="U12" s="65"/>
+      <c r="V12" s="65"/>
+      <c r="W12" s="66"/>
       <c r="X12" s="1"/>
       <c r="Y12" s="1"/>
     </row>
@@ -1773,17 +1890,17 @@
       <c r="J13" s="18">
         <v>1</v>
       </c>
-      <c r="M13" s="54"/>
-      <c r="N13" s="55"/>
-      <c r="O13" s="55"/>
-      <c r="P13" s="55"/>
-      <c r="Q13" s="55"/>
-      <c r="R13" s="55"/>
-      <c r="S13" s="55"/>
-      <c r="T13" s="55"/>
-      <c r="U13" s="55"/>
-      <c r="V13" s="55"/>
-      <c r="W13" s="56"/>
+      <c r="M13" s="67"/>
+      <c r="N13" s="68"/>
+      <c r="O13" s="68"/>
+      <c r="P13" s="68"/>
+      <c r="Q13" s="68"/>
+      <c r="R13" s="68"/>
+      <c r="S13" s="68"/>
+      <c r="T13" s="68"/>
+      <c r="U13" s="68"/>
+      <c r="V13" s="68"/>
+      <c r="W13" s="69"/>
       <c r="X13" s="1"/>
       <c r="Y13" s="1"/>
     </row>
@@ -1915,17 +2032,17 @@
       <c r="Y20" s="1"/>
     </row>
     <row r="21" spans="2:25" ht="24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="60" t="s">
+      <c r="B21" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="61"/>
-      <c r="D21" s="61"/>
-      <c r="E21" s="61"/>
-      <c r="F21" s="61"/>
-      <c r="G21" s="61"/>
-      <c r="H21" s="61"/>
-      <c r="I21" s="61"/>
-      <c r="J21" s="62"/>
+      <c r="C21" s="47"/>
+      <c r="D21" s="47"/>
+      <c r="E21" s="47"/>
+      <c r="F21" s="47"/>
+      <c r="G21" s="47"/>
+      <c r="H21" s="47"/>
+      <c r="I21" s="47"/>
+      <c r="J21" s="48"/>
       <c r="M21" s="33" t="s">
         <v>27</v>
       </c>
@@ -1933,53 +2050,53 @@
         <v>28</v>
       </c>
       <c r="O21" s="34"/>
-      <c r="P21" s="57" t="s">
+      <c r="P21" s="70" t="s">
         <v>46</v>
       </c>
-      <c r="Q21" s="57"/>
-      <c r="R21" s="57"/>
-      <c r="S21" s="57"/>
-      <c r="T21" s="57"/>
-      <c r="U21" s="57"/>
-      <c r="V21" s="57"/>
-      <c r="W21" s="58"/>
+      <c r="Q21" s="70"/>
+      <c r="R21" s="70"/>
+      <c r="S21" s="70"/>
+      <c r="T21" s="70"/>
+      <c r="U21" s="70"/>
+      <c r="V21" s="70"/>
+      <c r="W21" s="71"/>
       <c r="X21" s="1"/>
       <c r="Y21" s="1"/>
     </row>
     <row r="22" spans="2:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="63" t="s">
+      <c r="B22" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="65" t="s">
+      <c r="C22" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="D22" s="65" t="s">
+      <c r="D22" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="E22" s="65" t="s">
+      <c r="E22" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="F22" s="65" t="s">
+      <c r="F22" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="G22" s="67" t="s">
+      <c r="G22" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="H22" s="69" t="s">
+      <c r="H22" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="I22" s="70"/>
-      <c r="J22" s="71"/>
+      <c r="I22" s="56"/>
+      <c r="J22" s="57"/>
       <c r="X22" s="1"/>
       <c r="Y22" s="1"/>
     </row>
     <row r="23" spans="2:25" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="64"/>
-      <c r="C23" s="66"/>
-      <c r="D23" s="66"/>
-      <c r="E23" s="66"/>
-      <c r="F23" s="66"/>
-      <c r="G23" s="68"/>
+      <c r="B23" s="50"/>
+      <c r="C23" s="52"/>
+      <c r="D23" s="52"/>
+      <c r="E23" s="52"/>
+      <c r="F23" s="52"/>
+      <c r="G23" s="54"/>
       <c r="H23" s="14" t="s">
         <v>14</v>
       </c>
@@ -1989,19 +2106,17 @@
       <c r="J23" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="M23" s="48" t="s">
-        <v>61</v>
-      </c>
-      <c r="N23" s="49"/>
-      <c r="O23" s="49"/>
-      <c r="P23" s="49"/>
-      <c r="Q23" s="49"/>
-      <c r="R23" s="49"/>
-      <c r="S23" s="49"/>
-      <c r="T23" s="49"/>
-      <c r="U23" s="49"/>
-      <c r="V23" s="49"/>
-      <c r="W23" s="50"/>
+      <c r="M23" s="61"/>
+      <c r="N23" s="62"/>
+      <c r="O23" s="62"/>
+      <c r="P23" s="62"/>
+      <c r="Q23" s="62"/>
+      <c r="R23" s="62"/>
+      <c r="S23" s="62"/>
+      <c r="T23" s="62"/>
+      <c r="U23" s="62"/>
+      <c r="V23" s="62"/>
+      <c r="W23" s="63"/>
       <c r="X23" s="1"/>
       <c r="Y23" s="1"/>
     </row>
@@ -2015,17 +2130,17 @@
       <c r="H24" s="15"/>
       <c r="I24" s="9"/>
       <c r="J24" s="10"/>
-      <c r="M24" s="51"/>
-      <c r="N24" s="52"/>
-      <c r="O24" s="52"/>
-      <c r="P24" s="52"/>
-      <c r="Q24" s="52"/>
-      <c r="R24" s="52"/>
-      <c r="S24" s="52"/>
-      <c r="T24" s="52"/>
-      <c r="U24" s="52"/>
-      <c r="V24" s="52"/>
-      <c r="W24" s="53"/>
+      <c r="M24" s="64"/>
+      <c r="N24" s="65"/>
+      <c r="O24" s="65"/>
+      <c r="P24" s="65"/>
+      <c r="Q24" s="65"/>
+      <c r="R24" s="65"/>
+      <c r="S24" s="65"/>
+      <c r="T24" s="65"/>
+      <c r="U24" s="65"/>
+      <c r="V24" s="65"/>
+      <c r="W24" s="66"/>
     </row>
     <row r="25" spans="2:25" ht="30" x14ac:dyDescent="0.25">
       <c r="B25" s="8" t="s">
@@ -2047,17 +2162,17 @@
         <v>1</v>
       </c>
       <c r="J25" s="18"/>
-      <c r="M25" s="51"/>
-      <c r="N25" s="52"/>
-      <c r="O25" s="52"/>
-      <c r="P25" s="52"/>
-      <c r="Q25" s="52"/>
-      <c r="R25" s="52"/>
-      <c r="S25" s="52"/>
-      <c r="T25" s="52"/>
-      <c r="U25" s="52"/>
-      <c r="V25" s="52"/>
-      <c r="W25" s="53"/>
+      <c r="M25" s="64"/>
+      <c r="N25" s="65"/>
+      <c r="O25" s="65"/>
+      <c r="P25" s="65"/>
+      <c r="Q25" s="65"/>
+      <c r="R25" s="65"/>
+      <c r="S25" s="65"/>
+      <c r="T25" s="65"/>
+      <c r="U25" s="65"/>
+      <c r="V25" s="65"/>
+      <c r="W25" s="66"/>
     </row>
     <row r="26" spans="2:25" ht="30" x14ac:dyDescent="0.25">
       <c r="B26" s="8" t="s">
@@ -2079,17 +2194,17 @@
       </c>
       <c r="I26" s="17"/>
       <c r="J26" s="18"/>
-      <c r="M26" s="51"/>
-      <c r="N26" s="52"/>
-      <c r="O26" s="52"/>
-      <c r="P26" s="52"/>
-      <c r="Q26" s="52"/>
-      <c r="R26" s="52"/>
-      <c r="S26" s="52"/>
-      <c r="T26" s="52"/>
-      <c r="U26" s="52"/>
-      <c r="V26" s="52"/>
-      <c r="W26" s="53"/>
+      <c r="M26" s="64"/>
+      <c r="N26" s="65"/>
+      <c r="O26" s="65"/>
+      <c r="P26" s="65"/>
+      <c r="Q26" s="65"/>
+      <c r="R26" s="65"/>
+      <c r="S26" s="65"/>
+      <c r="T26" s="65"/>
+      <c r="U26" s="65"/>
+      <c r="V26" s="65"/>
+      <c r="W26" s="66"/>
     </row>
     <row r="27" spans="2:25" ht="30" x14ac:dyDescent="0.25">
       <c r="B27" s="8" t="s">
@@ -2111,17 +2226,17 @@
       </c>
       <c r="I27" s="17"/>
       <c r="J27" s="18"/>
-      <c r="M27" s="51"/>
-      <c r="N27" s="52"/>
-      <c r="O27" s="52"/>
-      <c r="P27" s="52"/>
-      <c r="Q27" s="52"/>
-      <c r="R27" s="52"/>
-      <c r="S27" s="52"/>
-      <c r="T27" s="52"/>
-      <c r="U27" s="52"/>
-      <c r="V27" s="52"/>
-      <c r="W27" s="53"/>
+      <c r="M27" s="64"/>
+      <c r="N27" s="65"/>
+      <c r="O27" s="65"/>
+      <c r="P27" s="65"/>
+      <c r="Q27" s="65"/>
+      <c r="R27" s="65"/>
+      <c r="S27" s="65"/>
+      <c r="T27" s="65"/>
+      <c r="U27" s="65"/>
+      <c r="V27" s="65"/>
+      <c r="W27" s="66"/>
     </row>
     <row r="28" spans="2:25" ht="45" x14ac:dyDescent="0.25">
       <c r="B28" s="8" t="s">
@@ -2143,17 +2258,17 @@
       </c>
       <c r="I28" s="17"/>
       <c r="J28" s="18"/>
-      <c r="M28" s="51"/>
-      <c r="N28" s="52"/>
-      <c r="O28" s="52"/>
-      <c r="P28" s="52"/>
-      <c r="Q28" s="52"/>
-      <c r="R28" s="52"/>
-      <c r="S28" s="52"/>
-      <c r="T28" s="52"/>
-      <c r="U28" s="52"/>
-      <c r="V28" s="52"/>
-      <c r="W28" s="53"/>
+      <c r="M28" s="64"/>
+      <c r="N28" s="65"/>
+      <c r="O28" s="65"/>
+      <c r="P28" s="65"/>
+      <c r="Q28" s="65"/>
+      <c r="R28" s="65"/>
+      <c r="S28" s="65"/>
+      <c r="T28" s="65"/>
+      <c r="U28" s="65"/>
+      <c r="V28" s="65"/>
+      <c r="W28" s="66"/>
     </row>
     <row r="29" spans="2:25" ht="30" x14ac:dyDescent="0.25">
       <c r="B29" s="8" t="s">
@@ -2175,17 +2290,17 @@
       </c>
       <c r="I29" s="17"/>
       <c r="J29" s="18"/>
-      <c r="M29" s="51"/>
-      <c r="N29" s="52"/>
-      <c r="O29" s="52"/>
-      <c r="P29" s="52"/>
-      <c r="Q29" s="52"/>
-      <c r="R29" s="52"/>
-      <c r="S29" s="52"/>
-      <c r="T29" s="52"/>
-      <c r="U29" s="52"/>
-      <c r="V29" s="52"/>
-      <c r="W29" s="53"/>
+      <c r="M29" s="64"/>
+      <c r="N29" s="65"/>
+      <c r="O29" s="65"/>
+      <c r="P29" s="65"/>
+      <c r="Q29" s="65"/>
+      <c r="R29" s="65"/>
+      <c r="S29" s="65"/>
+      <c r="T29" s="65"/>
+      <c r="U29" s="65"/>
+      <c r="V29" s="65"/>
+      <c r="W29" s="66"/>
     </row>
     <row r="30" spans="2:25" ht="30" x14ac:dyDescent="0.25">
       <c r="B30" s="8" t="s">
@@ -2207,17 +2322,17 @@
       <c r="J30" s="18">
         <v>1</v>
       </c>
-      <c r="M30" s="51"/>
-      <c r="N30" s="52"/>
-      <c r="O30" s="52"/>
-      <c r="P30" s="52"/>
-      <c r="Q30" s="52"/>
-      <c r="R30" s="52"/>
-      <c r="S30" s="52"/>
-      <c r="T30" s="52"/>
-      <c r="U30" s="52"/>
-      <c r="V30" s="52"/>
-      <c r="W30" s="53"/>
+      <c r="M30" s="64"/>
+      <c r="N30" s="65"/>
+      <c r="O30" s="65"/>
+      <c r="P30" s="65"/>
+      <c r="Q30" s="65"/>
+      <c r="R30" s="65"/>
+      <c r="S30" s="65"/>
+      <c r="T30" s="65"/>
+      <c r="U30" s="65"/>
+      <c r="V30" s="65"/>
+      <c r="W30" s="66"/>
     </row>
     <row r="31" spans="2:25" ht="30" x14ac:dyDescent="0.25">
       <c r="B31" s="8" t="s">
@@ -2241,17 +2356,17 @@
         <v>1</v>
       </c>
       <c r="J31" s="18"/>
-      <c r="M31" s="51"/>
-      <c r="N31" s="52"/>
-      <c r="O31" s="52"/>
-      <c r="P31" s="52"/>
-      <c r="Q31" s="52"/>
-      <c r="R31" s="52"/>
-      <c r="S31" s="52"/>
-      <c r="T31" s="52"/>
-      <c r="U31" s="52"/>
-      <c r="V31" s="52"/>
-      <c r="W31" s="53"/>
+      <c r="M31" s="64"/>
+      <c r="N31" s="65"/>
+      <c r="O31" s="65"/>
+      <c r="P31" s="65"/>
+      <c r="Q31" s="65"/>
+      <c r="R31" s="65"/>
+      <c r="S31" s="65"/>
+      <c r="T31" s="65"/>
+      <c r="U31" s="65"/>
+      <c r="V31" s="65"/>
+      <c r="W31" s="66"/>
     </row>
     <row r="32" spans="2:25" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="8" t="s">
@@ -2273,17 +2388,17 @@
       <c r="J32" s="18">
         <v>1</v>
       </c>
-      <c r="M32" s="54"/>
-      <c r="N32" s="55"/>
-      <c r="O32" s="55"/>
-      <c r="P32" s="55"/>
-      <c r="Q32" s="55"/>
-      <c r="R32" s="55"/>
-      <c r="S32" s="55"/>
-      <c r="T32" s="55"/>
-      <c r="U32" s="55"/>
-      <c r="V32" s="55"/>
-      <c r="W32" s="56"/>
+      <c r="M32" s="67"/>
+      <c r="N32" s="68"/>
+      <c r="O32" s="68"/>
+      <c r="P32" s="68"/>
+      <c r="Q32" s="68"/>
+      <c r="R32" s="68"/>
+      <c r="S32" s="68"/>
+      <c r="T32" s="68"/>
+      <c r="U32" s="68"/>
+      <c r="V32" s="68"/>
+      <c r="W32" s="69"/>
     </row>
     <row r="33" spans="2:23" ht="30" x14ac:dyDescent="0.25">
       <c r="B33" s="8" t="s">
@@ -2419,17 +2534,17 @@
     </row>
     <row r="43" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="44" spans="2:23" ht="24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="60" t="s">
+      <c r="B44" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="C44" s="61"/>
-      <c r="D44" s="61"/>
-      <c r="E44" s="61"/>
-      <c r="F44" s="61"/>
-      <c r="G44" s="61"/>
-      <c r="H44" s="61"/>
-      <c r="I44" s="61"/>
-      <c r="J44" s="62"/>
+      <c r="C44" s="47"/>
+      <c r="D44" s="47"/>
+      <c r="E44" s="47"/>
+      <c r="F44" s="47"/>
+      <c r="G44" s="47"/>
+      <c r="H44" s="47"/>
+      <c r="I44" s="47"/>
+      <c r="J44" s="48"/>
       <c r="M44" s="33" t="s">
         <v>27</v>
       </c>
@@ -2437,49 +2552,49 @@
         <v>28</v>
       </c>
       <c r="O44" s="34"/>
-      <c r="P44" s="57" t="s">
+      <c r="P44" s="70" t="s">
         <v>46</v>
       </c>
-      <c r="Q44" s="57"/>
-      <c r="R44" s="57"/>
-      <c r="S44" s="57"/>
-      <c r="T44" s="57"/>
-      <c r="U44" s="57"/>
-      <c r="V44" s="57"/>
-      <c r="W44" s="58"/>
+      <c r="Q44" s="70"/>
+      <c r="R44" s="70"/>
+      <c r="S44" s="70"/>
+      <c r="T44" s="70"/>
+      <c r="U44" s="70"/>
+      <c r="V44" s="70"/>
+      <c r="W44" s="71"/>
     </row>
     <row r="45" spans="2:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="63" t="s">
+      <c r="B45" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="C45" s="65" t="s">
+      <c r="C45" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="D45" s="65" t="s">
+      <c r="D45" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="E45" s="65" t="s">
+      <c r="E45" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="F45" s="65" t="s">
+      <c r="F45" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="G45" s="67" t="s">
+      <c r="G45" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="H45" s="69" t="s">
+      <c r="H45" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="I45" s="70"/>
-      <c r="J45" s="71"/>
+      <c r="I45" s="56"/>
+      <c r="J45" s="57"/>
     </row>
     <row r="46" spans="2:23" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="64"/>
-      <c r="C46" s="66"/>
-      <c r="D46" s="66"/>
-      <c r="E46" s="66"/>
-      <c r="F46" s="66"/>
-      <c r="G46" s="68"/>
+      <c r="B46" s="50"/>
+      <c r="C46" s="52"/>
+      <c r="D46" s="52"/>
+      <c r="E46" s="52"/>
+      <c r="F46" s="52"/>
+      <c r="G46" s="54"/>
       <c r="H46" s="14" t="s">
         <v>14</v>
       </c>
@@ -2489,19 +2604,19 @@
       <c r="J46" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="M46" s="48" t="s">
+      <c r="M46" s="61" t="s">
         <v>69</v>
       </c>
-      <c r="N46" s="49"/>
-      <c r="O46" s="49"/>
-      <c r="P46" s="49"/>
-      <c r="Q46" s="49"/>
-      <c r="R46" s="49"/>
-      <c r="S46" s="49"/>
-      <c r="T46" s="49"/>
-      <c r="U46" s="49"/>
-      <c r="V46" s="49"/>
-      <c r="W46" s="50"/>
+      <c r="N46" s="62"/>
+      <c r="O46" s="62"/>
+      <c r="P46" s="62"/>
+      <c r="Q46" s="62"/>
+      <c r="R46" s="62"/>
+      <c r="S46" s="62"/>
+      <c r="T46" s="62"/>
+      <c r="U46" s="62"/>
+      <c r="V46" s="62"/>
+      <c r="W46" s="63"/>
     </row>
     <row r="47" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B47" s="11"/>
@@ -2513,17 +2628,17 @@
       <c r="H47" s="15"/>
       <c r="I47" s="9"/>
       <c r="J47" s="10"/>
-      <c r="M47" s="51"/>
-      <c r="N47" s="52"/>
-      <c r="O47" s="52"/>
-      <c r="P47" s="52"/>
-      <c r="Q47" s="52"/>
-      <c r="R47" s="52"/>
-      <c r="S47" s="52"/>
-      <c r="T47" s="52"/>
-      <c r="U47" s="52"/>
-      <c r="V47" s="52"/>
-      <c r="W47" s="53"/>
+      <c r="M47" s="64"/>
+      <c r="N47" s="65"/>
+      <c r="O47" s="65"/>
+      <c r="P47" s="65"/>
+      <c r="Q47" s="65"/>
+      <c r="R47" s="65"/>
+      <c r="S47" s="65"/>
+      <c r="T47" s="65"/>
+      <c r="U47" s="65"/>
+      <c r="V47" s="65"/>
+      <c r="W47" s="66"/>
     </row>
     <row r="48" spans="2:23" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="8" t="s">
@@ -2543,17 +2658,17 @@
       </c>
       <c r="I48" s="17"/>
       <c r="J48" s="18"/>
-      <c r="M48" s="51"/>
-      <c r="N48" s="52"/>
-      <c r="O48" s="52"/>
-      <c r="P48" s="52"/>
-      <c r="Q48" s="52"/>
-      <c r="R48" s="52"/>
-      <c r="S48" s="52"/>
-      <c r="T48" s="52"/>
-      <c r="U48" s="52"/>
-      <c r="V48" s="52"/>
-      <c r="W48" s="53"/>
+      <c r="M48" s="64"/>
+      <c r="N48" s="65"/>
+      <c r="O48" s="65"/>
+      <c r="P48" s="65"/>
+      <c r="Q48" s="65"/>
+      <c r="R48" s="65"/>
+      <c r="S48" s="65"/>
+      <c r="T48" s="65"/>
+      <c r="U48" s="65"/>
+      <c r="V48" s="65"/>
+      <c r="W48" s="66"/>
     </row>
     <row r="49" spans="2:23" ht="30" x14ac:dyDescent="0.25">
       <c r="B49" s="8" t="s">
@@ -2573,17 +2688,17 @@
       </c>
       <c r="I49" s="17"/>
       <c r="J49" s="18"/>
-      <c r="M49" s="51"/>
-      <c r="N49" s="52"/>
-      <c r="O49" s="52"/>
-      <c r="P49" s="52"/>
-      <c r="Q49" s="52"/>
-      <c r="R49" s="52"/>
-      <c r="S49" s="52"/>
-      <c r="T49" s="52"/>
-      <c r="U49" s="52"/>
-      <c r="V49" s="52"/>
-      <c r="W49" s="53"/>
+      <c r="M49" s="64"/>
+      <c r="N49" s="65"/>
+      <c r="O49" s="65"/>
+      <c r="P49" s="65"/>
+      <c r="Q49" s="65"/>
+      <c r="R49" s="65"/>
+      <c r="S49" s="65"/>
+      <c r="T49" s="65"/>
+      <c r="U49" s="65"/>
+      <c r="V49" s="65"/>
+      <c r="W49" s="66"/>
     </row>
     <row r="50" spans="2:23" ht="30" x14ac:dyDescent="0.25">
       <c r="B50" s="8" t="s">
@@ -2605,17 +2720,17 @@
         <v>1</v>
       </c>
       <c r="J50" s="18"/>
-      <c r="M50" s="51"/>
-      <c r="N50" s="52"/>
-      <c r="O50" s="52"/>
-      <c r="P50" s="52"/>
-      <c r="Q50" s="52"/>
-      <c r="R50" s="52"/>
-      <c r="S50" s="52"/>
-      <c r="T50" s="52"/>
-      <c r="U50" s="52"/>
-      <c r="V50" s="52"/>
-      <c r="W50" s="53"/>
+      <c r="M50" s="64"/>
+      <c r="N50" s="65"/>
+      <c r="O50" s="65"/>
+      <c r="P50" s="65"/>
+      <c r="Q50" s="65"/>
+      <c r="R50" s="65"/>
+      <c r="S50" s="65"/>
+      <c r="T50" s="65"/>
+      <c r="U50" s="65"/>
+      <c r="V50" s="65"/>
+      <c r="W50" s="66"/>
     </row>
     <row r="51" spans="2:23" ht="30" x14ac:dyDescent="0.25">
       <c r="B51" s="8" t="s">
@@ -2635,17 +2750,17 @@
       </c>
       <c r="I51" s="17"/>
       <c r="J51" s="18"/>
-      <c r="M51" s="51"/>
-      <c r="N51" s="52"/>
-      <c r="O51" s="52"/>
-      <c r="P51" s="52"/>
-      <c r="Q51" s="52"/>
-      <c r="R51" s="52"/>
-      <c r="S51" s="52"/>
-      <c r="T51" s="52"/>
-      <c r="U51" s="52"/>
-      <c r="V51" s="52"/>
-      <c r="W51" s="53"/>
+      <c r="M51" s="64"/>
+      <c r="N51" s="65"/>
+      <c r="O51" s="65"/>
+      <c r="P51" s="65"/>
+      <c r="Q51" s="65"/>
+      <c r="R51" s="65"/>
+      <c r="S51" s="65"/>
+      <c r="T51" s="65"/>
+      <c r="U51" s="65"/>
+      <c r="V51" s="65"/>
+      <c r="W51" s="66"/>
     </row>
     <row r="52" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B52" s="4"/>
@@ -2657,30 +2772,30 @@
       <c r="H52" s="19"/>
       <c r="I52" s="20"/>
       <c r="J52" s="21"/>
-      <c r="M52" s="51"/>
-      <c r="N52" s="52"/>
-      <c r="O52" s="52"/>
-      <c r="P52" s="52"/>
-      <c r="Q52" s="52"/>
-      <c r="R52" s="52"/>
-      <c r="S52" s="52"/>
-      <c r="T52" s="52"/>
-      <c r="U52" s="52"/>
-      <c r="V52" s="52"/>
-      <c r="W52" s="53"/>
+      <c r="M52" s="64"/>
+      <c r="N52" s="65"/>
+      <c r="O52" s="65"/>
+      <c r="P52" s="65"/>
+      <c r="Q52" s="65"/>
+      <c r="R52" s="65"/>
+      <c r="S52" s="65"/>
+      <c r="T52" s="65"/>
+      <c r="U52" s="65"/>
+      <c r="V52" s="65"/>
+      <c r="W52" s="66"/>
     </row>
     <row r="53" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="M53" s="51"/>
-      <c r="N53" s="52"/>
-      <c r="O53" s="52"/>
-      <c r="P53" s="52"/>
-      <c r="Q53" s="52"/>
-      <c r="R53" s="52"/>
-      <c r="S53" s="52"/>
-      <c r="T53" s="52"/>
-      <c r="U53" s="52"/>
-      <c r="V53" s="52"/>
-      <c r="W53" s="53"/>
+      <c r="M53" s="64"/>
+      <c r="N53" s="65"/>
+      <c r="O53" s="65"/>
+      <c r="P53" s="65"/>
+      <c r="Q53" s="65"/>
+      <c r="R53" s="65"/>
+      <c r="S53" s="65"/>
+      <c r="T53" s="65"/>
+      <c r="U53" s="65"/>
+      <c r="V53" s="65"/>
+      <c r="W53" s="66"/>
     </row>
     <row r="54" spans="2:23" x14ac:dyDescent="0.25">
       <c r="G54" s="30" t="s">
@@ -2698,17 +2813,17 @@
         <f>SUM(J47:J52)</f>
         <v>0</v>
       </c>
-      <c r="M54" s="51"/>
-      <c r="N54" s="52"/>
-      <c r="O54" s="52"/>
-      <c r="P54" s="52"/>
-      <c r="Q54" s="52"/>
-      <c r="R54" s="52"/>
-      <c r="S54" s="52"/>
-      <c r="T54" s="52"/>
-      <c r="U54" s="52"/>
-      <c r="V54" s="52"/>
-      <c r="W54" s="53"/>
+      <c r="M54" s="64"/>
+      <c r="N54" s="65"/>
+      <c r="O54" s="65"/>
+      <c r="P54" s="65"/>
+      <c r="Q54" s="65"/>
+      <c r="R54" s="65"/>
+      <c r="S54" s="65"/>
+      <c r="T54" s="65"/>
+      <c r="U54" s="65"/>
+      <c r="V54" s="65"/>
+      <c r="W54" s="66"/>
     </row>
     <row r="55" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G55" s="31" t="s">
@@ -2726,35 +2841,35 @@
         <f>SUM(J48:J51)/ROWS(J48:J51)*100</f>
         <v>0</v>
       </c>
-      <c r="M55" s="54"/>
-      <c r="N55" s="55"/>
-      <c r="O55" s="55"/>
-      <c r="P55" s="55"/>
-      <c r="Q55" s="55"/>
-      <c r="R55" s="55"/>
-      <c r="S55" s="55"/>
-      <c r="T55" s="55"/>
-      <c r="U55" s="55"/>
-      <c r="V55" s="55"/>
-      <c r="W55" s="56"/>
+      <c r="M55" s="67"/>
+      <c r="N55" s="68"/>
+      <c r="O55" s="68"/>
+      <c r="P55" s="68"/>
+      <c r="Q55" s="68"/>
+      <c r="R55" s="68"/>
+      <c r="S55" s="68"/>
+      <c r="T55" s="68"/>
+      <c r="U55" s="68"/>
+      <c r="V55" s="68"/>
+      <c r="W55" s="69"/>
     </row>
     <row r="59" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="O59" s="59" t="s">
+      <c r="O59" s="72" t="s">
         <v>73</v>
       </c>
-      <c r="P59" s="59"/>
-      <c r="Q59" s="59"/>
-      <c r="R59" s="59"/>
-      <c r="S59" s="59"/>
+      <c r="P59" s="72"/>
+      <c r="Q59" s="72"/>
+      <c r="R59" s="72"/>
+      <c r="S59" s="72"/>
     </row>
     <row r="60" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="61" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G61" s="45" t="s">
+      <c r="G61" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="H61" s="46"/>
-      <c r="I61" s="46"/>
-      <c r="J61" s="47"/>
+      <c r="H61" s="59"/>
+      <c r="I61" s="59"/>
+      <c r="J61" s="60"/>
     </row>
     <row r="62" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G62" s="31" t="s">
@@ -2779,22 +2894,6 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="B21:J21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="H22:J22"/>
     <mergeCell ref="G61:J61"/>
     <mergeCell ref="M4:W13"/>
     <mergeCell ref="P2:W2"/>
@@ -2811,6 +2910,22 @@
     <mergeCell ref="F45:F46"/>
     <mergeCell ref="G45:G46"/>
     <mergeCell ref="H45:J45"/>
+    <mergeCell ref="B21:J21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="H22:J22"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:J3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Stand nach ersten ganzen druchlauf
</commit_message>
<xml_diff>
--- a/All_missions.xlsx
+++ b/All_missions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\silas\PycharmProjects\Robo_challenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E568DB6B-4F98-4D87-9D4D-39E41642BE68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED40FC8C-2181-40B0-8DF3-30DF207D9836}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="83">
   <si>
     <t>Main Tasks</t>
   </si>
@@ -306,111 +306,10 @@
     <t>unklar</t>
   </si>
   <si>
-    <t>gesicht muss etwa 7 cm nach object platziert sein und auf richtiger höhe…. Logging fehlt</t>
-  </si>
-  <si>
-    <t>find_face</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Speichern Sie relevante Informationen während der Fahrt in einer CSV-Datei (comma-separated-values) in geeigneten Datenstrukturen. 
-•	</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Erfassen Sie Zeitstempel für den Beginn der Fahrt, die Einfahrt in die Finisher-Box und für et-waige Wendemanöver.
-•	Berechnen Sie die Gesamtdauer Ihrer Fahrt von der Startposition bis zur Zielbox in Minuten und Sekunden (z. B. 5 Minuten 30 Sekunden). 
-•	Führen Sie Aufzeichnungen für jedes auf der Straße erkannte Objekt, einschließlich des Zeit-stempels der Erkennung. Zählen Sie auch die Gesamtzahl der erkannten Objekte.
-•	Führen Sie für jedes erkannte Gesicht einen Datensatz, der mindestens den Zeitstempel der Erkennung enthält. Verfolgen Sie auch die Gesamtzahl der erkannten Gesichter. Es gibt immer nur ein Gesicht pro Standort.</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-•	</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Führen Sie einen Datensatz für jedes Objekt und jeden QR-Code, den Sie während der Fahrt erkannt haben. Speichern Sie mindestens die folgenden Informationen pro Objekt: Zeitstempel, wann ein QR-Code gelesen wurde, Informationen, die Sie gelesen/gelesen haben, Aktion, die Sie durchgeführt haben. </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-•	</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Erfassen Sie, wann Sie einen (rechteckigen) Kreisverkehr betreten und verlassen haben.</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-•	</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Der QR-Code für den Spinntrick wurde geparst und in der CSV-Datei mit einem Zeitstempel protokolliert.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-•	Speichern Sie am Ende des Laufs die Kartendaten in einer separaten CSV-Datei.
-•	Speichern Sie andere Informationen, die Sie für wichtig halten.</t>
-    </r>
+    <t>SG/ST/RL</t>
+  </si>
+  <si>
+    <t>Kartendaten</t>
   </si>
 </sst>
 </file>
@@ -420,7 +319,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -464,22 +363,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="5"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1073,6 +956,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1108,51 +1036,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1496,37 +1379,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:Y62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="G17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23:W32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="8.140625" customWidth="1"/>
-    <col min="3" max="3" width="22.5703125" customWidth="1"/>
+    <col min="2" max="2" width="8.1796875" customWidth="1"/>
+    <col min="3" max="3" width="22.54296875" customWidth="1"/>
     <col min="4" max="4" width="8" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="6.5703125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.453125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7265625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:25" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:25" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="46" t="s">
+    <row r="1" spans="2:25" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:25" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="48"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="63"/>
       <c r="M2" s="33" t="s">
         <v>27</v>
       </c>
@@ -1534,49 +1417,49 @@
         <v>28</v>
       </c>
       <c r="O2" s="34"/>
-      <c r="P2" s="70" t="s">
+      <c r="P2" s="58" t="s">
         <v>46</v>
       </c>
-      <c r="Q2" s="70"/>
-      <c r="R2" s="70"/>
-      <c r="S2" s="70"/>
-      <c r="T2" s="70"/>
-      <c r="U2" s="70"/>
-      <c r="V2" s="70"/>
-      <c r="W2" s="71"/>
-    </row>
-    <row r="3" spans="2:25" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="49" t="s">
+      <c r="Q2" s="58"/>
+      <c r="R2" s="58"/>
+      <c r="S2" s="58"/>
+      <c r="T2" s="58"/>
+      <c r="U2" s="58"/>
+      <c r="V2" s="58"/>
+      <c r="W2" s="59"/>
+    </row>
+    <row r="3" spans="2:25" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="51" t="s">
+      <c r="C3" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="51" t="s">
+      <c r="D3" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="51" t="s">
+      <c r="E3" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="51" t="s">
+      <c r="F3" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="53" t="s">
+      <c r="G3" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="55" t="s">
+      <c r="H3" s="70" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="56"/>
-      <c r="J3" s="57"/>
-    </row>
-    <row r="4" spans="2:25" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="50"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="54"/>
+      <c r="I3" s="71"/>
+      <c r="J3" s="72"/>
+    </row>
+    <row r="4" spans="2:25" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="65"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="69"/>
       <c r="H4" s="14" t="s">
         <v>14</v>
       </c>
@@ -1586,23 +1469,23 @@
       <c r="J4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="61" t="s">
-        <v>83</v>
-      </c>
-      <c r="N4" s="62"/>
-      <c r="O4" s="62"/>
-      <c r="P4" s="62"/>
-      <c r="Q4" s="62"/>
-      <c r="R4" s="62"/>
-      <c r="S4" s="62"/>
-      <c r="T4" s="62"/>
-      <c r="U4" s="62"/>
-      <c r="V4" s="62"/>
-      <c r="W4" s="63"/>
+      <c r="M4" s="49" t="s">
+        <v>53</v>
+      </c>
+      <c r="N4" s="50"/>
+      <c r="O4" s="50"/>
+      <c r="P4" s="50"/>
+      <c r="Q4" s="50"/>
+      <c r="R4" s="50"/>
+      <c r="S4" s="50"/>
+      <c r="T4" s="50"/>
+      <c r="U4" s="50"/>
+      <c r="V4" s="50"/>
+      <c r="W4" s="51"/>
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
     </row>
-    <row r="5" spans="2:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="11"/>
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
@@ -1612,21 +1495,21 @@
       <c r="H5" s="15"/>
       <c r="I5" s="9"/>
       <c r="J5" s="10"/>
-      <c r="M5" s="64"/>
-      <c r="N5" s="65"/>
-      <c r="O5" s="65"/>
-      <c r="P5" s="65"/>
-      <c r="Q5" s="65"/>
-      <c r="R5" s="65"/>
-      <c r="S5" s="65"/>
-      <c r="T5" s="65"/>
-      <c r="U5" s="65"/>
-      <c r="V5" s="65"/>
-      <c r="W5" s="66"/>
+      <c r="M5" s="52"/>
+      <c r="N5" s="53"/>
+      <c r="O5" s="53"/>
+      <c r="P5" s="53"/>
+      <c r="Q5" s="53"/>
+      <c r="R5" s="53"/>
+      <c r="S5" s="53"/>
+      <c r="T5" s="53"/>
+      <c r="U5" s="53"/>
+      <c r="V5" s="53"/>
+      <c r="W5" s="54"/>
       <c r="X5" s="1"/>
       <c r="Y5" s="35"/>
     </row>
-    <row r="6" spans="2:25" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:25" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="37" t="s">
         <v>15</v>
       </c>
@@ -1646,21 +1529,21 @@
       </c>
       <c r="I6" s="42"/>
       <c r="J6" s="43"/>
-      <c r="M6" s="64"/>
-      <c r="N6" s="65"/>
-      <c r="O6" s="65"/>
-      <c r="P6" s="65"/>
-      <c r="Q6" s="65"/>
-      <c r="R6" s="65"/>
-      <c r="S6" s="65"/>
-      <c r="T6" s="65"/>
-      <c r="U6" s="65"/>
-      <c r="V6" s="65"/>
-      <c r="W6" s="66"/>
+      <c r="M6" s="52"/>
+      <c r="N6" s="53"/>
+      <c r="O6" s="53"/>
+      <c r="P6" s="53"/>
+      <c r="Q6" s="53"/>
+      <c r="R6" s="53"/>
+      <c r="S6" s="53"/>
+      <c r="T6" s="53"/>
+      <c r="U6" s="53"/>
+      <c r="V6" s="53"/>
+      <c r="W6" s="54"/>
       <c r="X6" s="1"/>
       <c r="Y6" s="1"/>
     </row>
-    <row r="7" spans="2:25" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:25" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="8" t="s">
         <v>15</v>
       </c>
@@ -1682,21 +1565,21 @@
         <v>1</v>
       </c>
       <c r="J7" s="43"/>
-      <c r="M7" s="64"/>
-      <c r="N7" s="65"/>
-      <c r="O7" s="65"/>
-      <c r="P7" s="65"/>
-      <c r="Q7" s="65"/>
-      <c r="R7" s="65"/>
-      <c r="S7" s="65"/>
-      <c r="T7" s="65"/>
-      <c r="U7" s="65"/>
-      <c r="V7" s="65"/>
-      <c r="W7" s="66"/>
+      <c r="M7" s="52"/>
+      <c r="N7" s="53"/>
+      <c r="O7" s="53"/>
+      <c r="P7" s="53"/>
+      <c r="Q7" s="53"/>
+      <c r="R7" s="53"/>
+      <c r="S7" s="53"/>
+      <c r="T7" s="53"/>
+      <c r="U7" s="53"/>
+      <c r="V7" s="53"/>
+      <c r="W7" s="54"/>
       <c r="X7" s="1"/>
       <c r="Y7" s="1"/>
     </row>
-    <row r="8" spans="2:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:25" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="37" t="s">
         <v>15</v>
       </c>
@@ -1708,31 +1591,31 @@
       </c>
       <c r="E8" s="40"/>
       <c r="F8" s="40" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="G8" s="45" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H8" s="41"/>
       <c r="I8" s="42">
         <v>1</v>
       </c>
       <c r="J8" s="43"/>
-      <c r="M8" s="64"/>
-      <c r="N8" s="65"/>
-      <c r="O8" s="65"/>
-      <c r="P8" s="65"/>
-      <c r="Q8" s="65"/>
-      <c r="R8" s="65"/>
-      <c r="S8" s="65"/>
-      <c r="T8" s="65"/>
-      <c r="U8" s="65"/>
-      <c r="V8" s="65"/>
-      <c r="W8" s="66"/>
+      <c r="M8" s="52"/>
+      <c r="N8" s="53"/>
+      <c r="O8" s="53"/>
+      <c r="P8" s="53"/>
+      <c r="Q8" s="53"/>
+      <c r="R8" s="53"/>
+      <c r="S8" s="53"/>
+      <c r="T8" s="53"/>
+      <c r="U8" s="53"/>
+      <c r="V8" s="53"/>
+      <c r="W8" s="54"/>
       <c r="X8" s="1"/>
       <c r="Y8" s="1"/>
     </row>
-    <row r="9" spans="2:25" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:25" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="8" t="s">
         <v>15</v>
       </c>
@@ -1754,21 +1637,21 @@
       </c>
       <c r="I9" s="17"/>
       <c r="J9" s="18"/>
-      <c r="M9" s="64"/>
-      <c r="N9" s="65"/>
-      <c r="O9" s="65"/>
-      <c r="P9" s="65"/>
-      <c r="Q9" s="65"/>
-      <c r="R9" s="65"/>
-      <c r="S9" s="65"/>
-      <c r="T9" s="65"/>
-      <c r="U9" s="65"/>
-      <c r="V9" s="65"/>
-      <c r="W9" s="66"/>
+      <c r="M9" s="52"/>
+      <c r="N9" s="53"/>
+      <c r="O9" s="53"/>
+      <c r="P9" s="53"/>
+      <c r="Q9" s="53"/>
+      <c r="R9" s="53"/>
+      <c r="S9" s="53"/>
+      <c r="T9" s="53"/>
+      <c r="U9" s="53"/>
+      <c r="V9" s="53"/>
+      <c r="W9" s="54"/>
       <c r="X9" s="1"/>
       <c r="Y9" s="1"/>
     </row>
-    <row r="10" spans="2:25" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:25" ht="42.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="8" t="s">
         <v>15</v>
       </c>
@@ -1788,21 +1671,21 @@
         <v>1</v>
       </c>
       <c r="J10" s="18"/>
-      <c r="M10" s="64"/>
-      <c r="N10" s="65"/>
-      <c r="O10" s="65"/>
-      <c r="P10" s="65"/>
-      <c r="Q10" s="65"/>
-      <c r="R10" s="65"/>
-      <c r="S10" s="65"/>
-      <c r="T10" s="65"/>
-      <c r="U10" s="65"/>
-      <c r="V10" s="65"/>
-      <c r="W10" s="66"/>
+      <c r="M10" s="52"/>
+      <c r="N10" s="53"/>
+      <c r="O10" s="53"/>
+      <c r="P10" s="53"/>
+      <c r="Q10" s="53"/>
+      <c r="R10" s="53"/>
+      <c r="S10" s="53"/>
+      <c r="T10" s="53"/>
+      <c r="U10" s="53"/>
+      <c r="V10" s="53"/>
+      <c r="W10" s="54"/>
       <c r="X10" s="1"/>
       <c r="Y10" s="1"/>
     </row>
-    <row r="11" spans="2:25" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:25" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="8" t="s">
         <v>15</v>
       </c>
@@ -1822,21 +1705,21 @@
       <c r="J11" s="18">
         <v>1</v>
       </c>
-      <c r="M11" s="64"/>
-      <c r="N11" s="65"/>
-      <c r="O11" s="65"/>
-      <c r="P11" s="65"/>
-      <c r="Q11" s="65"/>
-      <c r="R11" s="65"/>
-      <c r="S11" s="65"/>
-      <c r="T11" s="65"/>
-      <c r="U11" s="65"/>
-      <c r="V11" s="65"/>
-      <c r="W11" s="66"/>
+      <c r="M11" s="52"/>
+      <c r="N11" s="53"/>
+      <c r="O11" s="53"/>
+      <c r="P11" s="53"/>
+      <c r="Q11" s="53"/>
+      <c r="R11" s="53"/>
+      <c r="S11" s="53"/>
+      <c r="T11" s="53"/>
+      <c r="U11" s="53"/>
+      <c r="V11" s="53"/>
+      <c r="W11" s="54"/>
       <c r="X11" s="1"/>
       <c r="Y11" s="1"/>
     </row>
-    <row r="12" spans="2:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="8" t="s">
         <v>15</v>
       </c>
@@ -1851,26 +1734,26 @@
         <v>77</v>
       </c>
       <c r="G12" s="28"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="17">
+      <c r="H12" s="16">
         <v>1</v>
       </c>
+      <c r="I12" s="17"/>
       <c r="J12" s="18"/>
-      <c r="M12" s="64"/>
-      <c r="N12" s="65"/>
-      <c r="O12" s="65"/>
-      <c r="P12" s="65"/>
-      <c r="Q12" s="65"/>
-      <c r="R12" s="65"/>
-      <c r="S12" s="65"/>
-      <c r="T12" s="65"/>
-      <c r="U12" s="65"/>
-      <c r="V12" s="65"/>
-      <c r="W12" s="66"/>
+      <c r="M12" s="52"/>
+      <c r="N12" s="53"/>
+      <c r="O12" s="53"/>
+      <c r="P12" s="53"/>
+      <c r="Q12" s="53"/>
+      <c r="R12" s="53"/>
+      <c r="S12" s="53"/>
+      <c r="T12" s="53"/>
+      <c r="U12" s="53"/>
+      <c r="V12" s="53"/>
+      <c r="W12" s="54"/>
       <c r="X12" s="1"/>
       <c r="Y12" s="1"/>
     </row>
-    <row r="13" spans="2:25" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:25" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B13" s="8" t="s">
         <v>15</v>
       </c>
@@ -1890,21 +1773,21 @@
       <c r="J13" s="18">
         <v>1</v>
       </c>
-      <c r="M13" s="67"/>
-      <c r="N13" s="68"/>
-      <c r="O13" s="68"/>
-      <c r="P13" s="68"/>
-      <c r="Q13" s="68"/>
-      <c r="R13" s="68"/>
-      <c r="S13" s="68"/>
-      <c r="T13" s="68"/>
-      <c r="U13" s="68"/>
-      <c r="V13" s="68"/>
-      <c r="W13" s="69"/>
+      <c r="M13" s="55"/>
+      <c r="N13" s="56"/>
+      <c r="O13" s="56"/>
+      <c r="P13" s="56"/>
+      <c r="Q13" s="56"/>
+      <c r="R13" s="56"/>
+      <c r="S13" s="56"/>
+      <c r="T13" s="56"/>
+      <c r="U13" s="56"/>
+      <c r="V13" s="56"/>
+      <c r="W13" s="57"/>
       <c r="X13" s="1"/>
       <c r="Y13" s="1"/>
     </row>
-    <row r="14" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -1925,7 +1808,7 @@
       <c r="X14" s="1"/>
       <c r="Y14" s="1"/>
     </row>
-    <row r="15" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
@@ -1937,17 +1820,17 @@
       <c r="X15" s="1"/>
       <c r="Y15" s="1"/>
     </row>
-    <row r="16" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:25" x14ac:dyDescent="0.35">
       <c r="G16" s="30" t="s">
         <v>25</v>
       </c>
       <c r="H16" s="22">
         <f>SUM(H5:H14)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I16" s="23">
         <f>SUM(I5:I14)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J16" s="24">
         <f>SUM(J5:J14)</f>
@@ -1964,17 +1847,17 @@
       <c r="X16" s="1"/>
       <c r="Y16" s="1"/>
     </row>
-    <row r="17" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G17" s="31" t="s">
         <v>26</v>
       </c>
       <c r="H17" s="25">
         <f>SUM(H6:H13)/ROWS(H6:H13)*100</f>
-        <v>25</v>
+        <v>37.5</v>
       </c>
       <c r="I17" s="26">
         <f>SUM(I6:I13)/ROWS(I6:I13)*100</f>
-        <v>50</v>
+        <v>37.5</v>
       </c>
       <c r="J17" s="27">
         <f>SUM(J6:J13)/ROWS(J6:J13)*100</f>
@@ -1991,7 +1874,7 @@
       <c r="X17" s="1"/>
       <c r="Y17" s="1"/>
     </row>
-    <row r="18" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:25" x14ac:dyDescent="0.35">
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
@@ -2003,7 +1886,7 @@
       <c r="X18" s="1"/>
       <c r="Y18" s="1"/>
     </row>
-    <row r="19" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B19" s="3"/>
       <c r="C19" s="1"/>
       <c r="P19" s="1"/>
@@ -2017,7 +1900,7 @@
       <c r="X19" s="1"/>
       <c r="Y19" s="1"/>
     </row>
-    <row r="20" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B20" s="3"/>
       <c r="C20" s="1"/>
       <c r="P20" s="1"/>
@@ -2031,18 +1914,18 @@
       <c r="X20" s="1"/>
       <c r="Y20" s="1"/>
     </row>
-    <row r="21" spans="2:25" ht="24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="46" t="s">
+    <row r="21" spans="2:25" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B21" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="47"/>
-      <c r="D21" s="47"/>
-      <c r="E21" s="47"/>
-      <c r="F21" s="47"/>
-      <c r="G21" s="47"/>
-      <c r="H21" s="47"/>
-      <c r="I21" s="47"/>
-      <c r="J21" s="48"/>
+      <c r="C21" s="62"/>
+      <c r="D21" s="62"/>
+      <c r="E21" s="62"/>
+      <c r="F21" s="62"/>
+      <c r="G21" s="62"/>
+      <c r="H21" s="62"/>
+      <c r="I21" s="62"/>
+      <c r="J21" s="63"/>
       <c r="M21" s="33" t="s">
         <v>27</v>
       </c>
@@ -2050,53 +1933,53 @@
         <v>28</v>
       </c>
       <c r="O21" s="34"/>
-      <c r="P21" s="70" t="s">
+      <c r="P21" s="58" t="s">
         <v>46</v>
       </c>
-      <c r="Q21" s="70"/>
-      <c r="R21" s="70"/>
-      <c r="S21" s="70"/>
-      <c r="T21" s="70"/>
-      <c r="U21" s="70"/>
-      <c r="V21" s="70"/>
-      <c r="W21" s="71"/>
+      <c r="Q21" s="58"/>
+      <c r="R21" s="58"/>
+      <c r="S21" s="58"/>
+      <c r="T21" s="58"/>
+      <c r="U21" s="58"/>
+      <c r="V21" s="58"/>
+      <c r="W21" s="59"/>
       <c r="X21" s="1"/>
       <c r="Y21" s="1"/>
     </row>
-    <row r="22" spans="2:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="49" t="s">
+    <row r="22" spans="2:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B22" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="51" t="s">
+      <c r="C22" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="D22" s="51" t="s">
+      <c r="D22" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="E22" s="51" t="s">
+      <c r="E22" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="F22" s="51" t="s">
+      <c r="F22" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="G22" s="53" t="s">
+      <c r="G22" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="H22" s="55" t="s">
+      <c r="H22" s="70" t="s">
         <v>10</v>
       </c>
-      <c r="I22" s="56"/>
-      <c r="J22" s="57"/>
+      <c r="I22" s="71"/>
+      <c r="J22" s="72"/>
       <c r="X22" s="1"/>
       <c r="Y22" s="1"/>
     </row>
-    <row r="23" spans="2:25" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="50"/>
-      <c r="C23" s="52"/>
-      <c r="D23" s="52"/>
-      <c r="E23" s="52"/>
-      <c r="F23" s="52"/>
-      <c r="G23" s="54"/>
+    <row r="23" spans="2:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B23" s="65"/>
+      <c r="C23" s="67"/>
+      <c r="D23" s="67"/>
+      <c r="E23" s="67"/>
+      <c r="F23" s="67"/>
+      <c r="G23" s="69"/>
       <c r="H23" s="14" t="s">
         <v>14</v>
       </c>
@@ -2106,21 +1989,23 @@
       <c r="J23" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="M23" s="61"/>
-      <c r="N23" s="62"/>
-      <c r="O23" s="62"/>
-      <c r="P23" s="62"/>
-      <c r="Q23" s="62"/>
-      <c r="R23" s="62"/>
-      <c r="S23" s="62"/>
-      <c r="T23" s="62"/>
-      <c r="U23" s="62"/>
-      <c r="V23" s="62"/>
-      <c r="W23" s="63"/>
+      <c r="M23" s="49" t="s">
+        <v>59</v>
+      </c>
+      <c r="N23" s="50"/>
+      <c r="O23" s="50"/>
+      <c r="P23" s="50"/>
+      <c r="Q23" s="50"/>
+      <c r="R23" s="50"/>
+      <c r="S23" s="50"/>
+      <c r="T23" s="50"/>
+      <c r="U23" s="50"/>
+      <c r="V23" s="50"/>
+      <c r="W23" s="51"/>
       <c r="X23" s="1"/>
       <c r="Y23" s="1"/>
     </row>
-    <row r="24" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B24" s="11"/>
       <c r="C24" s="12"/>
       <c r="D24" s="12"/>
@@ -2130,19 +2015,19 @@
       <c r="H24" s="15"/>
       <c r="I24" s="9"/>
       <c r="J24" s="10"/>
-      <c r="M24" s="64"/>
-      <c r="N24" s="65"/>
-      <c r="O24" s="65"/>
-      <c r="P24" s="65"/>
-      <c r="Q24" s="65"/>
-      <c r="R24" s="65"/>
-      <c r="S24" s="65"/>
-      <c r="T24" s="65"/>
-      <c r="U24" s="65"/>
-      <c r="V24" s="65"/>
-      <c r="W24" s="66"/>
-    </row>
-    <row r="25" spans="2:25" ht="30" x14ac:dyDescent="0.25">
+      <c r="M24" s="52"/>
+      <c r="N24" s="53"/>
+      <c r="O24" s="53"/>
+      <c r="P24" s="53"/>
+      <c r="Q24" s="53"/>
+      <c r="R24" s="53"/>
+      <c r="S24" s="53"/>
+      <c r="T24" s="53"/>
+      <c r="U24" s="53"/>
+      <c r="V24" s="53"/>
+      <c r="W24" s="54"/>
+    </row>
+    <row r="25" spans="2:25" ht="29" x14ac:dyDescent="0.35">
       <c r="B25" s="8" t="s">
         <v>30</v>
       </c>
@@ -2157,24 +2042,24 @@
         <v>77</v>
       </c>
       <c r="G25" s="28"/>
-      <c r="H25" s="16"/>
-      <c r="I25" s="17">
+      <c r="H25" s="16">
         <v>1</v>
       </c>
+      <c r="I25" s="17"/>
       <c r="J25" s="18"/>
-      <c r="M25" s="64"/>
-      <c r="N25" s="65"/>
-      <c r="O25" s="65"/>
-      <c r="P25" s="65"/>
-      <c r="Q25" s="65"/>
-      <c r="R25" s="65"/>
-      <c r="S25" s="65"/>
-      <c r="T25" s="65"/>
-      <c r="U25" s="65"/>
-      <c r="V25" s="65"/>
-      <c r="W25" s="66"/>
-    </row>
-    <row r="26" spans="2:25" ht="30" x14ac:dyDescent="0.25">
+      <c r="M25" s="52"/>
+      <c r="N25" s="53"/>
+      <c r="O25" s="53"/>
+      <c r="P25" s="53"/>
+      <c r="Q25" s="53"/>
+      <c r="R25" s="53"/>
+      <c r="S25" s="53"/>
+      <c r="T25" s="53"/>
+      <c r="U25" s="53"/>
+      <c r="V25" s="53"/>
+      <c r="W25" s="54"/>
+    </row>
+    <row r="26" spans="2:25" ht="29" x14ac:dyDescent="0.35">
       <c r="B26" s="8" t="s">
         <v>30</v>
       </c>
@@ -2194,19 +2079,19 @@
       </c>
       <c r="I26" s="17"/>
       <c r="J26" s="18"/>
-      <c r="M26" s="64"/>
-      <c r="N26" s="65"/>
-      <c r="O26" s="65"/>
-      <c r="P26" s="65"/>
-      <c r="Q26" s="65"/>
-      <c r="R26" s="65"/>
-      <c r="S26" s="65"/>
-      <c r="T26" s="65"/>
-      <c r="U26" s="65"/>
-      <c r="V26" s="65"/>
-      <c r="W26" s="66"/>
-    </row>
-    <row r="27" spans="2:25" ht="30" x14ac:dyDescent="0.25">
+      <c r="M26" s="52"/>
+      <c r="N26" s="53"/>
+      <c r="O26" s="53"/>
+      <c r="P26" s="53"/>
+      <c r="Q26" s="53"/>
+      <c r="R26" s="53"/>
+      <c r="S26" s="53"/>
+      <c r="T26" s="53"/>
+      <c r="U26" s="53"/>
+      <c r="V26" s="53"/>
+      <c r="W26" s="54"/>
+    </row>
+    <row r="27" spans="2:25" ht="29" x14ac:dyDescent="0.35">
       <c r="B27" s="8" t="s">
         <v>30</v>
       </c>
@@ -2226,19 +2111,19 @@
       </c>
       <c r="I27" s="17"/>
       <c r="J27" s="18"/>
-      <c r="M27" s="64"/>
-      <c r="N27" s="65"/>
-      <c r="O27" s="65"/>
-      <c r="P27" s="65"/>
-      <c r="Q27" s="65"/>
-      <c r="R27" s="65"/>
-      <c r="S27" s="65"/>
-      <c r="T27" s="65"/>
-      <c r="U27" s="65"/>
-      <c r="V27" s="65"/>
-      <c r="W27" s="66"/>
-    </row>
-    <row r="28" spans="2:25" ht="45" x14ac:dyDescent="0.25">
+      <c r="M27" s="52"/>
+      <c r="N27" s="53"/>
+      <c r="O27" s="53"/>
+      <c r="P27" s="53"/>
+      <c r="Q27" s="53"/>
+      <c r="R27" s="53"/>
+      <c r="S27" s="53"/>
+      <c r="T27" s="53"/>
+      <c r="U27" s="53"/>
+      <c r="V27" s="53"/>
+      <c r="W27" s="54"/>
+    </row>
+    <row r="28" spans="2:25" ht="29" x14ac:dyDescent="0.35">
       <c r="B28" s="8" t="s">
         <v>30</v>
       </c>
@@ -2258,19 +2143,19 @@
       </c>
       <c r="I28" s="17"/>
       <c r="J28" s="18"/>
-      <c r="M28" s="64"/>
-      <c r="N28" s="65"/>
-      <c r="O28" s="65"/>
-      <c r="P28" s="65"/>
-      <c r="Q28" s="65"/>
-      <c r="R28" s="65"/>
-      <c r="S28" s="65"/>
-      <c r="T28" s="65"/>
-      <c r="U28" s="65"/>
-      <c r="V28" s="65"/>
-      <c r="W28" s="66"/>
-    </row>
-    <row r="29" spans="2:25" ht="30" x14ac:dyDescent="0.25">
+      <c r="M28" s="52"/>
+      <c r="N28" s="53"/>
+      <c r="O28" s="53"/>
+      <c r="P28" s="53"/>
+      <c r="Q28" s="53"/>
+      <c r="R28" s="53"/>
+      <c r="S28" s="53"/>
+      <c r="T28" s="53"/>
+      <c r="U28" s="53"/>
+      <c r="V28" s="53"/>
+      <c r="W28" s="54"/>
+    </row>
+    <row r="29" spans="2:25" ht="29" x14ac:dyDescent="0.35">
       <c r="B29" s="8" t="s">
         <v>30</v>
       </c>
@@ -2290,19 +2175,19 @@
       </c>
       <c r="I29" s="17"/>
       <c r="J29" s="18"/>
-      <c r="M29" s="64"/>
-      <c r="N29" s="65"/>
-      <c r="O29" s="65"/>
-      <c r="P29" s="65"/>
-      <c r="Q29" s="65"/>
-      <c r="R29" s="65"/>
-      <c r="S29" s="65"/>
-      <c r="T29" s="65"/>
-      <c r="U29" s="65"/>
-      <c r="V29" s="65"/>
-      <c r="W29" s="66"/>
-    </row>
-    <row r="30" spans="2:25" ht="30" x14ac:dyDescent="0.25">
+      <c r="M29" s="52"/>
+      <c r="N29" s="53"/>
+      <c r="O29" s="53"/>
+      <c r="P29" s="53"/>
+      <c r="Q29" s="53"/>
+      <c r="R29" s="53"/>
+      <c r="S29" s="53"/>
+      <c r="T29" s="53"/>
+      <c r="U29" s="53"/>
+      <c r="V29" s="53"/>
+      <c r="W29" s="54"/>
+    </row>
+    <row r="30" spans="2:25" ht="29" x14ac:dyDescent="0.35">
       <c r="B30" s="8" t="s">
         <v>30</v>
       </c>
@@ -2322,19 +2207,19 @@
       <c r="J30" s="18">
         <v>1</v>
       </c>
-      <c r="M30" s="64"/>
-      <c r="N30" s="65"/>
-      <c r="O30" s="65"/>
-      <c r="P30" s="65"/>
-      <c r="Q30" s="65"/>
-      <c r="R30" s="65"/>
-      <c r="S30" s="65"/>
-      <c r="T30" s="65"/>
-      <c r="U30" s="65"/>
-      <c r="V30" s="65"/>
-      <c r="W30" s="66"/>
-    </row>
-    <row r="31" spans="2:25" ht="30" x14ac:dyDescent="0.25">
+      <c r="M30" s="52"/>
+      <c r="N30" s="53"/>
+      <c r="O30" s="53"/>
+      <c r="P30" s="53"/>
+      <c r="Q30" s="53"/>
+      <c r="R30" s="53"/>
+      <c r="S30" s="53"/>
+      <c r="T30" s="53"/>
+      <c r="U30" s="53"/>
+      <c r="V30" s="53"/>
+      <c r="W30" s="54"/>
+    </row>
+    <row r="31" spans="2:25" ht="29" x14ac:dyDescent="0.35">
       <c r="B31" s="8" t="s">
         <v>30</v>
       </c>
@@ -2344,31 +2229,29 @@
       <c r="D31" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="E31" s="28" t="s">
-        <v>82</v>
-      </c>
+      <c r="E31" s="28"/>
       <c r="F31" s="28" t="s">
         <v>77</v>
       </c>
       <c r="G31" s="28"/>
-      <c r="H31" s="16"/>
-      <c r="I31" s="17">
+      <c r="H31" s="16">
         <v>1</v>
       </c>
+      <c r="I31" s="17"/>
       <c r="J31" s="18"/>
-      <c r="M31" s="64"/>
-      <c r="N31" s="65"/>
-      <c r="O31" s="65"/>
-      <c r="P31" s="65"/>
-      <c r="Q31" s="65"/>
-      <c r="R31" s="65"/>
-      <c r="S31" s="65"/>
-      <c r="T31" s="65"/>
-      <c r="U31" s="65"/>
-      <c r="V31" s="65"/>
-      <c r="W31" s="66"/>
-    </row>
-    <row r="32" spans="2:25" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M31" s="52"/>
+      <c r="N31" s="53"/>
+      <c r="O31" s="53"/>
+      <c r="P31" s="53"/>
+      <c r="Q31" s="53"/>
+      <c r="R31" s="53"/>
+      <c r="S31" s="53"/>
+      <c r="T31" s="53"/>
+      <c r="U31" s="53"/>
+      <c r="V31" s="53"/>
+      <c r="W31" s="54"/>
+    </row>
+    <row r="32" spans="2:25" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B32" s="8" t="s">
         <v>30</v>
       </c>
@@ -2388,19 +2271,19 @@
       <c r="J32" s="18">
         <v>1</v>
       </c>
-      <c r="M32" s="67"/>
-      <c r="N32" s="68"/>
-      <c r="O32" s="68"/>
-      <c r="P32" s="68"/>
-      <c r="Q32" s="68"/>
-      <c r="R32" s="68"/>
-      <c r="S32" s="68"/>
-      <c r="T32" s="68"/>
-      <c r="U32" s="68"/>
-      <c r="V32" s="68"/>
-      <c r="W32" s="69"/>
-    </row>
-    <row r="33" spans="2:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="M32" s="55"/>
+      <c r="N32" s="56"/>
+      <c r="O32" s="56"/>
+      <c r="P32" s="56"/>
+      <c r="Q32" s="56"/>
+      <c r="R32" s="56"/>
+      <c r="S32" s="56"/>
+      <c r="T32" s="56"/>
+      <c r="U32" s="56"/>
+      <c r="V32" s="56"/>
+      <c r="W32" s="57"/>
+    </row>
+    <row r="33" spans="2:23" ht="29" x14ac:dyDescent="0.35">
       <c r="B33" s="8" t="s">
         <v>30</v>
       </c>
@@ -2421,7 +2304,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="2:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:23" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B34" s="8" t="s">
         <v>30</v>
       </c>
@@ -2436,13 +2319,13 @@
         <v>77</v>
       </c>
       <c r="G34" s="28"/>
-      <c r="H34" s="16"/>
-      <c r="I34" s="17">
+      <c r="H34" s="16">
         <v>1</v>
       </c>
+      <c r="I34" s="17"/>
       <c r="J34" s="18"/>
     </row>
-    <row r="35" spans="2:23" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:23" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B35" s="8" t="s">
         <v>30</v>
       </c>
@@ -2465,7 +2348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="2:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:23" ht="29" x14ac:dyDescent="0.35">
       <c r="B36" s="8" t="s">
         <v>30</v>
       </c>
@@ -2486,7 +2369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B37" s="4"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
@@ -2497,54 +2380,54 @@
       <c r="I37" s="20"/>
       <c r="J37" s="21"/>
     </row>
-    <row r="38" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="39" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="39" spans="2:23" x14ac:dyDescent="0.35">
       <c r="G39" s="30" t="s">
         <v>25</v>
       </c>
       <c r="H39" s="22">
         <f>SUM(H24:H37)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I39" s="23">
         <f>SUM(I24:I37)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J39" s="24">
         <f>SUM(J24:J37)</f>
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G40" s="31" t="s">
         <v>26</v>
       </c>
       <c r="H40" s="25">
         <f>SUM(H25:H36)/ROWS(H25:H36)*100</f>
-        <v>33.333333333333329</v>
+        <v>58.333333333333336</v>
       </c>
       <c r="I40" s="26">
         <f>SUM(I25:I36)/ROWS(I25:I36)*100</f>
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="J40" s="27">
         <f>SUM(J25:J36)/ROWS(J25:J36)*100</f>
         <v>41.666666666666671</v>
       </c>
     </row>
-    <row r="43" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="44" spans="2:23" ht="24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="46" t="s">
+    <row r="43" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="44" spans="2:23" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B44" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="C44" s="47"/>
-      <c r="D44" s="47"/>
-      <c r="E44" s="47"/>
-      <c r="F44" s="47"/>
-      <c r="G44" s="47"/>
-      <c r="H44" s="47"/>
-      <c r="I44" s="47"/>
-      <c r="J44" s="48"/>
+      <c r="C44" s="62"/>
+      <c r="D44" s="62"/>
+      <c r="E44" s="62"/>
+      <c r="F44" s="62"/>
+      <c r="G44" s="62"/>
+      <c r="H44" s="62"/>
+      <c r="I44" s="62"/>
+      <c r="J44" s="63"/>
       <c r="M44" s="33" t="s">
         <v>27</v>
       </c>
@@ -2552,49 +2435,49 @@
         <v>28</v>
       </c>
       <c r="O44" s="34"/>
-      <c r="P44" s="70" t="s">
+      <c r="P44" s="58" t="s">
         <v>46</v>
       </c>
-      <c r="Q44" s="70"/>
-      <c r="R44" s="70"/>
-      <c r="S44" s="70"/>
-      <c r="T44" s="70"/>
-      <c r="U44" s="70"/>
-      <c r="V44" s="70"/>
-      <c r="W44" s="71"/>
-    </row>
-    <row r="45" spans="2:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="49" t="s">
+      <c r="Q44" s="58"/>
+      <c r="R44" s="58"/>
+      <c r="S44" s="58"/>
+      <c r="T44" s="58"/>
+      <c r="U44" s="58"/>
+      <c r="V44" s="58"/>
+      <c r="W44" s="59"/>
+    </row>
+    <row r="45" spans="2:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B45" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="C45" s="51" t="s">
+      <c r="C45" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="D45" s="51" t="s">
+      <c r="D45" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="E45" s="51" t="s">
+      <c r="E45" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="F45" s="51" t="s">
+      <c r="F45" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="G45" s="53" t="s">
+      <c r="G45" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="H45" s="55" t="s">
+      <c r="H45" s="70" t="s">
         <v>10</v>
       </c>
-      <c r="I45" s="56"/>
-      <c r="J45" s="57"/>
-    </row>
-    <row r="46" spans="2:23" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="50"/>
-      <c r="C46" s="52"/>
-      <c r="D46" s="52"/>
-      <c r="E46" s="52"/>
-      <c r="F46" s="52"/>
-      <c r="G46" s="54"/>
+      <c r="I45" s="71"/>
+      <c r="J45" s="72"/>
+    </row>
+    <row r="46" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B46" s="65"/>
+      <c r="C46" s="67"/>
+      <c r="D46" s="67"/>
+      <c r="E46" s="67"/>
+      <c r="F46" s="67"/>
+      <c r="G46" s="69"/>
       <c r="H46" s="14" t="s">
         <v>14</v>
       </c>
@@ -2604,21 +2487,21 @@
       <c r="J46" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="M46" s="61" t="s">
+      <c r="M46" s="49" t="s">
         <v>69</v>
       </c>
-      <c r="N46" s="62"/>
-      <c r="O46" s="62"/>
-      <c r="P46" s="62"/>
-      <c r="Q46" s="62"/>
-      <c r="R46" s="62"/>
-      <c r="S46" s="62"/>
-      <c r="T46" s="62"/>
-      <c r="U46" s="62"/>
-      <c r="V46" s="62"/>
-      <c r="W46" s="63"/>
-    </row>
-    <row r="47" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="N46" s="50"/>
+      <c r="O46" s="50"/>
+      <c r="P46" s="50"/>
+      <c r="Q46" s="50"/>
+      <c r="R46" s="50"/>
+      <c r="S46" s="50"/>
+      <c r="T46" s="50"/>
+      <c r="U46" s="50"/>
+      <c r="V46" s="50"/>
+      <c r="W46" s="51"/>
+    </row>
+    <row r="47" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B47" s="11"/>
       <c r="C47" s="12"/>
       <c r="D47" s="12"/>
@@ -2628,19 +2511,19 @@
       <c r="H47" s="15"/>
       <c r="I47" s="9"/>
       <c r="J47" s="10"/>
-      <c r="M47" s="64"/>
-      <c r="N47" s="65"/>
-      <c r="O47" s="65"/>
-      <c r="P47" s="65"/>
-      <c r="Q47" s="65"/>
-      <c r="R47" s="65"/>
-      <c r="S47" s="65"/>
-      <c r="T47" s="65"/>
-      <c r="U47" s="65"/>
-      <c r="V47" s="65"/>
-      <c r="W47" s="66"/>
-    </row>
-    <row r="48" spans="2:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="M47" s="52"/>
+      <c r="N47" s="53"/>
+      <c r="O47" s="53"/>
+      <c r="P47" s="53"/>
+      <c r="Q47" s="53"/>
+      <c r="R47" s="53"/>
+      <c r="S47" s="53"/>
+      <c r="T47" s="53"/>
+      <c r="U47" s="53"/>
+      <c r="V47" s="53"/>
+      <c r="W47" s="54"/>
+    </row>
+    <row r="48" spans="2:23" ht="29" x14ac:dyDescent="0.35">
       <c r="B48" s="8" t="s">
         <v>31</v>
       </c>
@@ -2658,19 +2541,19 @@
       </c>
       <c r="I48" s="17"/>
       <c r="J48" s="18"/>
-      <c r="M48" s="64"/>
-      <c r="N48" s="65"/>
-      <c r="O48" s="65"/>
-      <c r="P48" s="65"/>
-      <c r="Q48" s="65"/>
-      <c r="R48" s="65"/>
-      <c r="S48" s="65"/>
-      <c r="T48" s="65"/>
-      <c r="U48" s="65"/>
-      <c r="V48" s="65"/>
-      <c r="W48" s="66"/>
-    </row>
-    <row r="49" spans="2:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="M48" s="52"/>
+      <c r="N48" s="53"/>
+      <c r="O48" s="53"/>
+      <c r="P48" s="53"/>
+      <c r="Q48" s="53"/>
+      <c r="R48" s="53"/>
+      <c r="S48" s="53"/>
+      <c r="T48" s="53"/>
+      <c r="U48" s="53"/>
+      <c r="V48" s="53"/>
+      <c r="W48" s="54"/>
+    </row>
+    <row r="49" spans="2:23" ht="29" x14ac:dyDescent="0.35">
       <c r="B49" s="8" t="s">
         <v>31</v>
       </c>
@@ -2688,19 +2571,19 @@
       </c>
       <c r="I49" s="17"/>
       <c r="J49" s="18"/>
-      <c r="M49" s="64"/>
-      <c r="N49" s="65"/>
-      <c r="O49" s="65"/>
-      <c r="P49" s="65"/>
-      <c r="Q49" s="65"/>
-      <c r="R49" s="65"/>
-      <c r="S49" s="65"/>
-      <c r="T49" s="65"/>
-      <c r="U49" s="65"/>
-      <c r="V49" s="65"/>
-      <c r="W49" s="66"/>
-    </row>
-    <row r="50" spans="2:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="M49" s="52"/>
+      <c r="N49" s="53"/>
+      <c r="O49" s="53"/>
+      <c r="P49" s="53"/>
+      <c r="Q49" s="53"/>
+      <c r="R49" s="53"/>
+      <c r="S49" s="53"/>
+      <c r="T49" s="53"/>
+      <c r="U49" s="53"/>
+      <c r="V49" s="53"/>
+      <c r="W49" s="54"/>
+    </row>
+    <row r="50" spans="2:23" ht="29" x14ac:dyDescent="0.35">
       <c r="B50" s="8" t="s">
         <v>31</v>
       </c>
@@ -2720,19 +2603,19 @@
         <v>1</v>
       </c>
       <c r="J50" s="18"/>
-      <c r="M50" s="64"/>
-      <c r="N50" s="65"/>
-      <c r="O50" s="65"/>
-      <c r="P50" s="65"/>
-      <c r="Q50" s="65"/>
-      <c r="R50" s="65"/>
-      <c r="S50" s="65"/>
-      <c r="T50" s="65"/>
-      <c r="U50" s="65"/>
-      <c r="V50" s="65"/>
-      <c r="W50" s="66"/>
-    </row>
-    <row r="51" spans="2:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="M50" s="52"/>
+      <c r="N50" s="53"/>
+      <c r="O50" s="53"/>
+      <c r="P50" s="53"/>
+      <c r="Q50" s="53"/>
+      <c r="R50" s="53"/>
+      <c r="S50" s="53"/>
+      <c r="T50" s="53"/>
+      <c r="U50" s="53"/>
+      <c r="V50" s="53"/>
+      <c r="W50" s="54"/>
+    </row>
+    <row r="51" spans="2:23" ht="29" x14ac:dyDescent="0.35">
       <c r="B51" s="8" t="s">
         <v>31</v>
       </c>
@@ -2750,19 +2633,19 @@
       </c>
       <c r="I51" s="17"/>
       <c r="J51" s="18"/>
-      <c r="M51" s="64"/>
-      <c r="N51" s="65"/>
-      <c r="O51" s="65"/>
-      <c r="P51" s="65"/>
-      <c r="Q51" s="65"/>
-      <c r="R51" s="65"/>
-      <c r="S51" s="65"/>
-      <c r="T51" s="65"/>
-      <c r="U51" s="65"/>
-      <c r="V51" s="65"/>
-      <c r="W51" s="66"/>
-    </row>
-    <row r="52" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M51" s="52"/>
+      <c r="N51" s="53"/>
+      <c r="O51" s="53"/>
+      <c r="P51" s="53"/>
+      <c r="Q51" s="53"/>
+      <c r="R51" s="53"/>
+      <c r="S51" s="53"/>
+      <c r="T51" s="53"/>
+      <c r="U51" s="53"/>
+      <c r="V51" s="53"/>
+      <c r="W51" s="54"/>
+    </row>
+    <row r="52" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B52" s="4"/>
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
@@ -2772,32 +2655,32 @@
       <c r="H52" s="19"/>
       <c r="I52" s="20"/>
       <c r="J52" s="21"/>
-      <c r="M52" s="64"/>
-      <c r="N52" s="65"/>
-      <c r="O52" s="65"/>
-      <c r="P52" s="65"/>
-      <c r="Q52" s="65"/>
-      <c r="R52" s="65"/>
-      <c r="S52" s="65"/>
-      <c r="T52" s="65"/>
-      <c r="U52" s="65"/>
-      <c r="V52" s="65"/>
-      <c r="W52" s="66"/>
-    </row>
-    <row r="53" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="M53" s="64"/>
-      <c r="N53" s="65"/>
-      <c r="O53" s="65"/>
-      <c r="P53" s="65"/>
-      <c r="Q53" s="65"/>
-      <c r="R53" s="65"/>
-      <c r="S53" s="65"/>
-      <c r="T53" s="65"/>
-      <c r="U53" s="65"/>
-      <c r="V53" s="65"/>
-      <c r="W53" s="66"/>
-    </row>
-    <row r="54" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="M52" s="52"/>
+      <c r="N52" s="53"/>
+      <c r="O52" s="53"/>
+      <c r="P52" s="53"/>
+      <c r="Q52" s="53"/>
+      <c r="R52" s="53"/>
+      <c r="S52" s="53"/>
+      <c r="T52" s="53"/>
+      <c r="U52" s="53"/>
+      <c r="V52" s="53"/>
+      <c r="W52" s="54"/>
+    </row>
+    <row r="53" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="M53" s="52"/>
+      <c r="N53" s="53"/>
+      <c r="O53" s="53"/>
+      <c r="P53" s="53"/>
+      <c r="Q53" s="53"/>
+      <c r="R53" s="53"/>
+      <c r="S53" s="53"/>
+      <c r="T53" s="53"/>
+      <c r="U53" s="53"/>
+      <c r="V53" s="53"/>
+      <c r="W53" s="54"/>
+    </row>
+    <row r="54" spans="2:23" x14ac:dyDescent="0.35">
       <c r="G54" s="30" t="s">
         <v>25</v>
       </c>
@@ -2813,19 +2696,19 @@
         <f>SUM(J47:J52)</f>
         <v>0</v>
       </c>
-      <c r="M54" s="64"/>
-      <c r="N54" s="65"/>
-      <c r="O54" s="65"/>
-      <c r="P54" s="65"/>
-      <c r="Q54" s="65"/>
-      <c r="R54" s="65"/>
-      <c r="S54" s="65"/>
-      <c r="T54" s="65"/>
-      <c r="U54" s="65"/>
-      <c r="V54" s="65"/>
-      <c r="W54" s="66"/>
-    </row>
-    <row r="55" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M54" s="52"/>
+      <c r="N54" s="53"/>
+      <c r="O54" s="53"/>
+      <c r="P54" s="53"/>
+      <c r="Q54" s="53"/>
+      <c r="R54" s="53"/>
+      <c r="S54" s="53"/>
+      <c r="T54" s="53"/>
+      <c r="U54" s="53"/>
+      <c r="V54" s="53"/>
+      <c r="W54" s="54"/>
+    </row>
+    <row r="55" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G55" s="31" t="s">
         <v>26</v>
       </c>
@@ -2841,47 +2724,47 @@
         <f>SUM(J48:J51)/ROWS(J48:J51)*100</f>
         <v>0</v>
       </c>
-      <c r="M55" s="67"/>
-      <c r="N55" s="68"/>
-      <c r="O55" s="68"/>
-      <c r="P55" s="68"/>
-      <c r="Q55" s="68"/>
-      <c r="R55" s="68"/>
-      <c r="S55" s="68"/>
-      <c r="T55" s="68"/>
-      <c r="U55" s="68"/>
-      <c r="V55" s="68"/>
-      <c r="W55" s="69"/>
-    </row>
-    <row r="59" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="O59" s="72" t="s">
+      <c r="M55" s="55"/>
+      <c r="N55" s="56"/>
+      <c r="O55" s="56"/>
+      <c r="P55" s="56"/>
+      <c r="Q55" s="56"/>
+      <c r="R55" s="56"/>
+      <c r="S55" s="56"/>
+      <c r="T55" s="56"/>
+      <c r="U55" s="56"/>
+      <c r="V55" s="56"/>
+      <c r="W55" s="57"/>
+    </row>
+    <row r="59" spans="2:23" x14ac:dyDescent="0.35">
+      <c r="O59" s="60" t="s">
         <v>73</v>
       </c>
-      <c r="P59" s="72"/>
-      <c r="Q59" s="72"/>
-      <c r="R59" s="72"/>
-      <c r="S59" s="72"/>
-    </row>
-    <row r="60" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="61" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G61" s="58" t="s">
+      <c r="P59" s="60"/>
+      <c r="Q59" s="60"/>
+      <c r="R59" s="60"/>
+      <c r="S59" s="60"/>
+    </row>
+    <row r="60" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="61" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G61" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="H61" s="59"/>
-      <c r="I61" s="59"/>
-      <c r="J61" s="60"/>
-    </row>
-    <row r="62" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H61" s="47"/>
+      <c r="I61" s="47"/>
+      <c r="J61" s="48"/>
+    </row>
+    <row r="62" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G62" s="31" t="s">
         <v>26</v>
       </c>
       <c r="H62" s="25">
         <f>SUM(H17+H40+H55)/3</f>
-        <v>44.444444444444436</v>
+        <v>56.94444444444445</v>
       </c>
       <c r="I62" s="26">
         <f>SUM(I17+I40+I55)/3</f>
-        <v>33.333333333333336</v>
+        <v>20.833333333333332</v>
       </c>
       <c r="J62" s="27">
         <f>SUM(J17+J40+J55)/3</f>
@@ -2889,11 +2772,27 @@
       </c>
       <c r="K62" s="36">
         <f>SUM(H62:J62)</f>
-        <v>100</v>
+        <v>100.00000000000001</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="B21:J21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="H22:J22"/>
     <mergeCell ref="G61:J61"/>
     <mergeCell ref="M4:W13"/>
     <mergeCell ref="P2:W2"/>
@@ -2910,22 +2809,6 @@
     <mergeCell ref="F45:F46"/>
     <mergeCell ref="G45:G46"/>
     <mergeCell ref="H45:J45"/>
-    <mergeCell ref="B21:J21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="H22:J22"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="H3:J3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2940,7 +2823,7 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Stand nach zweitem ganzen druchlauf und Bild pushen
</commit_message>
<xml_diff>
--- a/All_missions.xlsx
+++ b/All_missions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\silas\PycharmProjects\Robo_challenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED40FC8C-2181-40B0-8DF3-30DF207D9836}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81EEB6C8-519D-4D22-879F-CF99AAA9812A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -956,6 +956,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1000,42 +1036,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1379,8 +1379,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:Y62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23:W32"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1399,17 +1399,17 @@
   <sheetData>
     <row r="1" spans="2:25" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:25" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="61" t="s">
+      <c r="B2" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="63"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="48"/>
       <c r="M2" s="33" t="s">
         <v>27</v>
       </c>
@@ -1417,49 +1417,49 @@
         <v>28</v>
       </c>
       <c r="O2" s="34"/>
-      <c r="P2" s="58" t="s">
+      <c r="P2" s="70" t="s">
         <v>46</v>
       </c>
-      <c r="Q2" s="58"/>
-      <c r="R2" s="58"/>
-      <c r="S2" s="58"/>
-      <c r="T2" s="58"/>
-      <c r="U2" s="58"/>
-      <c r="V2" s="58"/>
-      <c r="W2" s="59"/>
+      <c r="Q2" s="70"/>
+      <c r="R2" s="70"/>
+      <c r="S2" s="70"/>
+      <c r="T2" s="70"/>
+      <c r="U2" s="70"/>
+      <c r="V2" s="70"/>
+      <c r="W2" s="71"/>
     </row>
     <row r="3" spans="2:25" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="66" t="s">
+      <c r="C3" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="66" t="s">
+      <c r="D3" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="66" t="s">
+      <c r="E3" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="66" t="s">
+      <c r="F3" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="68" t="s">
+      <c r="G3" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="70" t="s">
+      <c r="H3" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="71"/>
-      <c r="J3" s="72"/>
+      <c r="I3" s="56"/>
+      <c r="J3" s="57"/>
     </row>
     <row r="4" spans="2:25" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="65"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="G4" s="69"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="54"/>
       <c r="H4" s="14" t="s">
         <v>14</v>
       </c>
@@ -1469,19 +1469,19 @@
       <c r="J4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="49" t="s">
-        <v>53</v>
-      </c>
-      <c r="N4" s="50"/>
-      <c r="O4" s="50"/>
-      <c r="P4" s="50"/>
-      <c r="Q4" s="50"/>
-      <c r="R4" s="50"/>
-      <c r="S4" s="50"/>
-      <c r="T4" s="50"/>
-      <c r="U4" s="50"/>
-      <c r="V4" s="50"/>
-      <c r="W4" s="51"/>
+      <c r="M4" s="61" t="s">
+        <v>47</v>
+      </c>
+      <c r="N4" s="62"/>
+      <c r="O4" s="62"/>
+      <c r="P4" s="62"/>
+      <c r="Q4" s="62"/>
+      <c r="R4" s="62"/>
+      <c r="S4" s="62"/>
+      <c r="T4" s="62"/>
+      <c r="U4" s="62"/>
+      <c r="V4" s="62"/>
+      <c r="W4" s="63"/>
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
     </row>
@@ -1495,17 +1495,17 @@
       <c r="H5" s="15"/>
       <c r="I5" s="9"/>
       <c r="J5" s="10"/>
-      <c r="M5" s="52"/>
-      <c r="N5" s="53"/>
-      <c r="O5" s="53"/>
-      <c r="P5" s="53"/>
-      <c r="Q5" s="53"/>
-      <c r="R5" s="53"/>
-      <c r="S5" s="53"/>
-      <c r="T5" s="53"/>
-      <c r="U5" s="53"/>
-      <c r="V5" s="53"/>
-      <c r="W5" s="54"/>
+      <c r="M5" s="64"/>
+      <c r="N5" s="65"/>
+      <c r="O5" s="65"/>
+      <c r="P5" s="65"/>
+      <c r="Q5" s="65"/>
+      <c r="R5" s="65"/>
+      <c r="S5" s="65"/>
+      <c r="T5" s="65"/>
+      <c r="U5" s="65"/>
+      <c r="V5" s="65"/>
+      <c r="W5" s="66"/>
       <c r="X5" s="1"/>
       <c r="Y5" s="35"/>
     </row>
@@ -1529,17 +1529,17 @@
       </c>
       <c r="I6" s="42"/>
       <c r="J6" s="43"/>
-      <c r="M6" s="52"/>
-      <c r="N6" s="53"/>
-      <c r="O6" s="53"/>
-      <c r="P6" s="53"/>
-      <c r="Q6" s="53"/>
-      <c r="R6" s="53"/>
-      <c r="S6" s="53"/>
-      <c r="T6" s="53"/>
-      <c r="U6" s="53"/>
-      <c r="V6" s="53"/>
-      <c r="W6" s="54"/>
+      <c r="M6" s="64"/>
+      <c r="N6" s="65"/>
+      <c r="O6" s="65"/>
+      <c r="P6" s="65"/>
+      <c r="Q6" s="65"/>
+      <c r="R6" s="65"/>
+      <c r="S6" s="65"/>
+      <c r="T6" s="65"/>
+      <c r="U6" s="65"/>
+      <c r="V6" s="65"/>
+      <c r="W6" s="66"/>
       <c r="X6" s="1"/>
       <c r="Y6" s="1"/>
     </row>
@@ -1560,22 +1560,22 @@
         <v>74</v>
       </c>
       <c r="G7" s="40"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="42">
+      <c r="H7" s="41">
         <v>1</v>
       </c>
+      <c r="I7" s="42"/>
       <c r="J7" s="43"/>
-      <c r="M7" s="52"/>
-      <c r="N7" s="53"/>
-      <c r="O7" s="53"/>
-      <c r="P7" s="53"/>
-      <c r="Q7" s="53"/>
-      <c r="R7" s="53"/>
-      <c r="S7" s="53"/>
-      <c r="T7" s="53"/>
-      <c r="U7" s="53"/>
-      <c r="V7" s="53"/>
-      <c r="W7" s="54"/>
+      <c r="M7" s="64"/>
+      <c r="N7" s="65"/>
+      <c r="O7" s="65"/>
+      <c r="P7" s="65"/>
+      <c r="Q7" s="65"/>
+      <c r="R7" s="65"/>
+      <c r="S7" s="65"/>
+      <c r="T7" s="65"/>
+      <c r="U7" s="65"/>
+      <c r="V7" s="65"/>
+      <c r="W7" s="66"/>
       <c r="X7" s="1"/>
       <c r="Y7" s="1"/>
     </row>
@@ -1601,17 +1601,17 @@
         <v>1</v>
       </c>
       <c r="J8" s="43"/>
-      <c r="M8" s="52"/>
-      <c r="N8" s="53"/>
-      <c r="O8" s="53"/>
-      <c r="P8" s="53"/>
-      <c r="Q8" s="53"/>
-      <c r="R8" s="53"/>
-      <c r="S8" s="53"/>
-      <c r="T8" s="53"/>
-      <c r="U8" s="53"/>
-      <c r="V8" s="53"/>
-      <c r="W8" s="54"/>
+      <c r="M8" s="64"/>
+      <c r="N8" s="65"/>
+      <c r="O8" s="65"/>
+      <c r="P8" s="65"/>
+      <c r="Q8" s="65"/>
+      <c r="R8" s="65"/>
+      <c r="S8" s="65"/>
+      <c r="T8" s="65"/>
+      <c r="U8" s="65"/>
+      <c r="V8" s="65"/>
+      <c r="W8" s="66"/>
       <c r="X8" s="1"/>
       <c r="Y8" s="1"/>
     </row>
@@ -1637,17 +1637,17 @@
       </c>
       <c r="I9" s="17"/>
       <c r="J9" s="18"/>
-      <c r="M9" s="52"/>
-      <c r="N9" s="53"/>
-      <c r="O9" s="53"/>
-      <c r="P9" s="53"/>
-      <c r="Q9" s="53"/>
-      <c r="R9" s="53"/>
-      <c r="S9" s="53"/>
-      <c r="T9" s="53"/>
-      <c r="U9" s="53"/>
-      <c r="V9" s="53"/>
-      <c r="W9" s="54"/>
+      <c r="M9" s="64"/>
+      <c r="N9" s="65"/>
+      <c r="O9" s="65"/>
+      <c r="P9" s="65"/>
+      <c r="Q9" s="65"/>
+      <c r="R9" s="65"/>
+      <c r="S9" s="65"/>
+      <c r="T9" s="65"/>
+      <c r="U9" s="65"/>
+      <c r="V9" s="65"/>
+      <c r="W9" s="66"/>
       <c r="X9" s="1"/>
       <c r="Y9" s="1"/>
     </row>
@@ -1671,17 +1671,17 @@
         <v>1</v>
       </c>
       <c r="J10" s="18"/>
-      <c r="M10" s="52"/>
-      <c r="N10" s="53"/>
-      <c r="O10" s="53"/>
-      <c r="P10" s="53"/>
-      <c r="Q10" s="53"/>
-      <c r="R10" s="53"/>
-      <c r="S10" s="53"/>
-      <c r="T10" s="53"/>
-      <c r="U10" s="53"/>
-      <c r="V10" s="53"/>
-      <c r="W10" s="54"/>
+      <c r="M10" s="64"/>
+      <c r="N10" s="65"/>
+      <c r="O10" s="65"/>
+      <c r="P10" s="65"/>
+      <c r="Q10" s="65"/>
+      <c r="R10" s="65"/>
+      <c r="S10" s="65"/>
+      <c r="T10" s="65"/>
+      <c r="U10" s="65"/>
+      <c r="V10" s="65"/>
+      <c r="W10" s="66"/>
       <c r="X10" s="1"/>
       <c r="Y10" s="1"/>
     </row>
@@ -1705,17 +1705,17 @@
       <c r="J11" s="18">
         <v>1</v>
       </c>
-      <c r="M11" s="52"/>
-      <c r="N11" s="53"/>
-      <c r="O11" s="53"/>
-      <c r="P11" s="53"/>
-      <c r="Q11" s="53"/>
-      <c r="R11" s="53"/>
-      <c r="S11" s="53"/>
-      <c r="T11" s="53"/>
-      <c r="U11" s="53"/>
-      <c r="V11" s="53"/>
-      <c r="W11" s="54"/>
+      <c r="M11" s="64"/>
+      <c r="N11" s="65"/>
+      <c r="O11" s="65"/>
+      <c r="P11" s="65"/>
+      <c r="Q11" s="65"/>
+      <c r="R11" s="65"/>
+      <c r="S11" s="65"/>
+      <c r="T11" s="65"/>
+      <c r="U11" s="65"/>
+      <c r="V11" s="65"/>
+      <c r="W11" s="66"/>
       <c r="X11" s="1"/>
       <c r="Y11" s="1"/>
     </row>
@@ -1739,17 +1739,17 @@
       </c>
       <c r="I12" s="17"/>
       <c r="J12" s="18"/>
-      <c r="M12" s="52"/>
-      <c r="N12" s="53"/>
-      <c r="O12" s="53"/>
-      <c r="P12" s="53"/>
-      <c r="Q12" s="53"/>
-      <c r="R12" s="53"/>
-      <c r="S12" s="53"/>
-      <c r="T12" s="53"/>
-      <c r="U12" s="53"/>
-      <c r="V12" s="53"/>
-      <c r="W12" s="54"/>
+      <c r="M12" s="64"/>
+      <c r="N12" s="65"/>
+      <c r="O12" s="65"/>
+      <c r="P12" s="65"/>
+      <c r="Q12" s="65"/>
+      <c r="R12" s="65"/>
+      <c r="S12" s="65"/>
+      <c r="T12" s="65"/>
+      <c r="U12" s="65"/>
+      <c r="V12" s="65"/>
+      <c r="W12" s="66"/>
       <c r="X12" s="1"/>
       <c r="Y12" s="1"/>
     </row>
@@ -1773,17 +1773,17 @@
       <c r="J13" s="18">
         <v>1</v>
       </c>
-      <c r="M13" s="55"/>
-      <c r="N13" s="56"/>
-      <c r="O13" s="56"/>
-      <c r="P13" s="56"/>
-      <c r="Q13" s="56"/>
-      <c r="R13" s="56"/>
-      <c r="S13" s="56"/>
-      <c r="T13" s="56"/>
-      <c r="U13" s="56"/>
-      <c r="V13" s="56"/>
-      <c r="W13" s="57"/>
+      <c r="M13" s="67"/>
+      <c r="N13" s="68"/>
+      <c r="O13" s="68"/>
+      <c r="P13" s="68"/>
+      <c r="Q13" s="68"/>
+      <c r="R13" s="68"/>
+      <c r="S13" s="68"/>
+      <c r="T13" s="68"/>
+      <c r="U13" s="68"/>
+      <c r="V13" s="68"/>
+      <c r="W13" s="69"/>
       <c r="X13" s="1"/>
       <c r="Y13" s="1"/>
     </row>
@@ -1826,11 +1826,11 @@
       </c>
       <c r="H16" s="22">
         <f>SUM(H5:H14)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I16" s="23">
         <f>SUM(I5:I14)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J16" s="24">
         <f>SUM(J5:J14)</f>
@@ -1853,11 +1853,11 @@
       </c>
       <c r="H17" s="25">
         <f>SUM(H6:H13)/ROWS(H6:H13)*100</f>
-        <v>37.5</v>
+        <v>50</v>
       </c>
       <c r="I17" s="26">
         <f>SUM(I6:I13)/ROWS(I6:I13)*100</f>
-        <v>37.5</v>
+        <v>25</v>
       </c>
       <c r="J17" s="27">
         <f>SUM(J6:J13)/ROWS(J6:J13)*100</f>
@@ -1915,17 +1915,17 @@
       <c r="Y20" s="1"/>
     </row>
     <row r="21" spans="2:25" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B21" s="61" t="s">
+      <c r="B21" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="62"/>
-      <c r="D21" s="62"/>
-      <c r="E21" s="62"/>
-      <c r="F21" s="62"/>
-      <c r="G21" s="62"/>
-      <c r="H21" s="62"/>
-      <c r="I21" s="62"/>
-      <c r="J21" s="63"/>
+      <c r="C21" s="47"/>
+      <c r="D21" s="47"/>
+      <c r="E21" s="47"/>
+      <c r="F21" s="47"/>
+      <c r="G21" s="47"/>
+      <c r="H21" s="47"/>
+      <c r="I21" s="47"/>
+      <c r="J21" s="48"/>
       <c r="M21" s="33" t="s">
         <v>27</v>
       </c>
@@ -1933,53 +1933,53 @@
         <v>28</v>
       </c>
       <c r="O21" s="34"/>
-      <c r="P21" s="58" t="s">
+      <c r="P21" s="70" t="s">
         <v>46</v>
       </c>
-      <c r="Q21" s="58"/>
-      <c r="R21" s="58"/>
-      <c r="S21" s="58"/>
-      <c r="T21" s="58"/>
-      <c r="U21" s="58"/>
-      <c r="V21" s="58"/>
-      <c r="W21" s="59"/>
+      <c r="Q21" s="70"/>
+      <c r="R21" s="70"/>
+      <c r="S21" s="70"/>
+      <c r="T21" s="70"/>
+      <c r="U21" s="70"/>
+      <c r="V21" s="70"/>
+      <c r="W21" s="71"/>
       <c r="X21" s="1"/>
       <c r="Y21" s="1"/>
     </row>
     <row r="22" spans="2:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B22" s="64" t="s">
+      <c r="B22" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="66" t="s">
+      <c r="C22" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="D22" s="66" t="s">
+      <c r="D22" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="E22" s="66" t="s">
+      <c r="E22" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="F22" s="66" t="s">
+      <c r="F22" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="G22" s="68" t="s">
+      <c r="G22" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="H22" s="70" t="s">
+      <c r="H22" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="I22" s="71"/>
-      <c r="J22" s="72"/>
+      <c r="I22" s="56"/>
+      <c r="J22" s="57"/>
       <c r="X22" s="1"/>
       <c r="Y22" s="1"/>
     </row>
     <row r="23" spans="2:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="65"/>
-      <c r="C23" s="67"/>
-      <c r="D23" s="67"/>
-      <c r="E23" s="67"/>
-      <c r="F23" s="67"/>
-      <c r="G23" s="69"/>
+      <c r="B23" s="50"/>
+      <c r="C23" s="52"/>
+      <c r="D23" s="52"/>
+      <c r="E23" s="52"/>
+      <c r="F23" s="52"/>
+      <c r="G23" s="54"/>
       <c r="H23" s="14" t="s">
         <v>14</v>
       </c>
@@ -1989,19 +1989,19 @@
       <c r="J23" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="M23" s="49" t="s">
+      <c r="M23" s="61" t="s">
         <v>59</v>
       </c>
-      <c r="N23" s="50"/>
-      <c r="O23" s="50"/>
-      <c r="P23" s="50"/>
-      <c r="Q23" s="50"/>
-      <c r="R23" s="50"/>
-      <c r="S23" s="50"/>
-      <c r="T23" s="50"/>
-      <c r="U23" s="50"/>
-      <c r="V23" s="50"/>
-      <c r="W23" s="51"/>
+      <c r="N23" s="62"/>
+      <c r="O23" s="62"/>
+      <c r="P23" s="62"/>
+      <c r="Q23" s="62"/>
+      <c r="R23" s="62"/>
+      <c r="S23" s="62"/>
+      <c r="T23" s="62"/>
+      <c r="U23" s="62"/>
+      <c r="V23" s="62"/>
+      <c r="W23" s="63"/>
       <c r="X23" s="1"/>
       <c r="Y23" s="1"/>
     </row>
@@ -2015,17 +2015,17 @@
       <c r="H24" s="15"/>
       <c r="I24" s="9"/>
       <c r="J24" s="10"/>
-      <c r="M24" s="52"/>
-      <c r="N24" s="53"/>
-      <c r="O24" s="53"/>
-      <c r="P24" s="53"/>
-      <c r="Q24" s="53"/>
-      <c r="R24" s="53"/>
-      <c r="S24" s="53"/>
-      <c r="T24" s="53"/>
-      <c r="U24" s="53"/>
-      <c r="V24" s="53"/>
-      <c r="W24" s="54"/>
+      <c r="M24" s="64"/>
+      <c r="N24" s="65"/>
+      <c r="O24" s="65"/>
+      <c r="P24" s="65"/>
+      <c r="Q24" s="65"/>
+      <c r="R24" s="65"/>
+      <c r="S24" s="65"/>
+      <c r="T24" s="65"/>
+      <c r="U24" s="65"/>
+      <c r="V24" s="65"/>
+      <c r="W24" s="66"/>
     </row>
     <row r="25" spans="2:25" ht="29" x14ac:dyDescent="0.35">
       <c r="B25" s="8" t="s">
@@ -2047,17 +2047,17 @@
       </c>
       <c r="I25" s="17"/>
       <c r="J25" s="18"/>
-      <c r="M25" s="52"/>
-      <c r="N25" s="53"/>
-      <c r="O25" s="53"/>
-      <c r="P25" s="53"/>
-      <c r="Q25" s="53"/>
-      <c r="R25" s="53"/>
-      <c r="S25" s="53"/>
-      <c r="T25" s="53"/>
-      <c r="U25" s="53"/>
-      <c r="V25" s="53"/>
-      <c r="W25" s="54"/>
+      <c r="M25" s="64"/>
+      <c r="N25" s="65"/>
+      <c r="O25" s="65"/>
+      <c r="P25" s="65"/>
+      <c r="Q25" s="65"/>
+      <c r="R25" s="65"/>
+      <c r="S25" s="65"/>
+      <c r="T25" s="65"/>
+      <c r="U25" s="65"/>
+      <c r="V25" s="65"/>
+      <c r="W25" s="66"/>
     </row>
     <row r="26" spans="2:25" ht="29" x14ac:dyDescent="0.35">
       <c r="B26" s="8" t="s">
@@ -2079,17 +2079,17 @@
       </c>
       <c r="I26" s="17"/>
       <c r="J26" s="18"/>
-      <c r="M26" s="52"/>
-      <c r="N26" s="53"/>
-      <c r="O26" s="53"/>
-      <c r="P26" s="53"/>
-      <c r="Q26" s="53"/>
-      <c r="R26" s="53"/>
-      <c r="S26" s="53"/>
-      <c r="T26" s="53"/>
-      <c r="U26" s="53"/>
-      <c r="V26" s="53"/>
-      <c r="W26" s="54"/>
+      <c r="M26" s="64"/>
+      <c r="N26" s="65"/>
+      <c r="O26" s="65"/>
+      <c r="P26" s="65"/>
+      <c r="Q26" s="65"/>
+      <c r="R26" s="65"/>
+      <c r="S26" s="65"/>
+      <c r="T26" s="65"/>
+      <c r="U26" s="65"/>
+      <c r="V26" s="65"/>
+      <c r="W26" s="66"/>
     </row>
     <row r="27" spans="2:25" ht="29" x14ac:dyDescent="0.35">
       <c r="B27" s="8" t="s">
@@ -2111,17 +2111,17 @@
       </c>
       <c r="I27" s="17"/>
       <c r="J27" s="18"/>
-      <c r="M27" s="52"/>
-      <c r="N27" s="53"/>
-      <c r="O27" s="53"/>
-      <c r="P27" s="53"/>
-      <c r="Q27" s="53"/>
-      <c r="R27" s="53"/>
-      <c r="S27" s="53"/>
-      <c r="T27" s="53"/>
-      <c r="U27" s="53"/>
-      <c r="V27" s="53"/>
-      <c r="W27" s="54"/>
+      <c r="M27" s="64"/>
+      <c r="N27" s="65"/>
+      <c r="O27" s="65"/>
+      <c r="P27" s="65"/>
+      <c r="Q27" s="65"/>
+      <c r="R27" s="65"/>
+      <c r="S27" s="65"/>
+      <c r="T27" s="65"/>
+      <c r="U27" s="65"/>
+      <c r="V27" s="65"/>
+      <c r="W27" s="66"/>
     </row>
     <row r="28" spans="2:25" ht="29" x14ac:dyDescent="0.35">
       <c r="B28" s="8" t="s">
@@ -2143,17 +2143,17 @@
       </c>
       <c r="I28" s="17"/>
       <c r="J28" s="18"/>
-      <c r="M28" s="52"/>
-      <c r="N28" s="53"/>
-      <c r="O28" s="53"/>
-      <c r="P28" s="53"/>
-      <c r="Q28" s="53"/>
-      <c r="R28" s="53"/>
-      <c r="S28" s="53"/>
-      <c r="T28" s="53"/>
-      <c r="U28" s="53"/>
-      <c r="V28" s="53"/>
-      <c r="W28" s="54"/>
+      <c r="M28" s="64"/>
+      <c r="N28" s="65"/>
+      <c r="O28" s="65"/>
+      <c r="P28" s="65"/>
+      <c r="Q28" s="65"/>
+      <c r="R28" s="65"/>
+      <c r="S28" s="65"/>
+      <c r="T28" s="65"/>
+      <c r="U28" s="65"/>
+      <c r="V28" s="65"/>
+      <c r="W28" s="66"/>
     </row>
     <row r="29" spans="2:25" ht="29" x14ac:dyDescent="0.35">
       <c r="B29" s="8" t="s">
@@ -2175,17 +2175,17 @@
       </c>
       <c r="I29" s="17"/>
       <c r="J29" s="18"/>
-      <c r="M29" s="52"/>
-      <c r="N29" s="53"/>
-      <c r="O29" s="53"/>
-      <c r="P29" s="53"/>
-      <c r="Q29" s="53"/>
-      <c r="R29" s="53"/>
-      <c r="S29" s="53"/>
-      <c r="T29" s="53"/>
-      <c r="U29" s="53"/>
-      <c r="V29" s="53"/>
-      <c r="W29" s="54"/>
+      <c r="M29" s="64"/>
+      <c r="N29" s="65"/>
+      <c r="O29" s="65"/>
+      <c r="P29" s="65"/>
+      <c r="Q29" s="65"/>
+      <c r="R29" s="65"/>
+      <c r="S29" s="65"/>
+      <c r="T29" s="65"/>
+      <c r="U29" s="65"/>
+      <c r="V29" s="65"/>
+      <c r="W29" s="66"/>
     </row>
     <row r="30" spans="2:25" ht="29" x14ac:dyDescent="0.35">
       <c r="B30" s="8" t="s">
@@ -2202,22 +2202,22 @@
         <v>77</v>
       </c>
       <c r="G30" s="28"/>
-      <c r="H30" s="16"/>
+      <c r="H30" s="16">
+        <v>1</v>
+      </c>
       <c r="I30" s="17"/>
-      <c r="J30" s="18">
-        <v>1</v>
-      </c>
-      <c r="M30" s="52"/>
-      <c r="N30" s="53"/>
-      <c r="O30" s="53"/>
-      <c r="P30" s="53"/>
-      <c r="Q30" s="53"/>
-      <c r="R30" s="53"/>
-      <c r="S30" s="53"/>
-      <c r="T30" s="53"/>
-      <c r="U30" s="53"/>
-      <c r="V30" s="53"/>
-      <c r="W30" s="54"/>
+      <c r="J30" s="18"/>
+      <c r="M30" s="64"/>
+      <c r="N30" s="65"/>
+      <c r="O30" s="65"/>
+      <c r="P30" s="65"/>
+      <c r="Q30" s="65"/>
+      <c r="R30" s="65"/>
+      <c r="S30" s="65"/>
+      <c r="T30" s="65"/>
+      <c r="U30" s="65"/>
+      <c r="V30" s="65"/>
+      <c r="W30" s="66"/>
     </row>
     <row r="31" spans="2:25" ht="29" x14ac:dyDescent="0.35">
       <c r="B31" s="8" t="s">
@@ -2239,17 +2239,17 @@
       </c>
       <c r="I31" s="17"/>
       <c r="J31" s="18"/>
-      <c r="M31" s="52"/>
-      <c r="N31" s="53"/>
-      <c r="O31" s="53"/>
-      <c r="P31" s="53"/>
-      <c r="Q31" s="53"/>
-      <c r="R31" s="53"/>
-      <c r="S31" s="53"/>
-      <c r="T31" s="53"/>
-      <c r="U31" s="53"/>
-      <c r="V31" s="53"/>
-      <c r="W31" s="54"/>
+      <c r="M31" s="64"/>
+      <c r="N31" s="65"/>
+      <c r="O31" s="65"/>
+      <c r="P31" s="65"/>
+      <c r="Q31" s="65"/>
+      <c r="R31" s="65"/>
+      <c r="S31" s="65"/>
+      <c r="T31" s="65"/>
+      <c r="U31" s="65"/>
+      <c r="V31" s="65"/>
+      <c r="W31" s="66"/>
     </row>
     <row r="32" spans="2:25" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B32" s="8" t="s">
@@ -2271,17 +2271,17 @@
       <c r="J32" s="18">
         <v>1</v>
       </c>
-      <c r="M32" s="55"/>
-      <c r="N32" s="56"/>
-      <c r="O32" s="56"/>
-      <c r="P32" s="56"/>
-      <c r="Q32" s="56"/>
-      <c r="R32" s="56"/>
-      <c r="S32" s="56"/>
-      <c r="T32" s="56"/>
-      <c r="U32" s="56"/>
-      <c r="V32" s="56"/>
-      <c r="W32" s="57"/>
+      <c r="M32" s="67"/>
+      <c r="N32" s="68"/>
+      <c r="O32" s="68"/>
+      <c r="P32" s="68"/>
+      <c r="Q32" s="68"/>
+      <c r="R32" s="68"/>
+      <c r="S32" s="68"/>
+      <c r="T32" s="68"/>
+      <c r="U32" s="68"/>
+      <c r="V32" s="68"/>
+      <c r="W32" s="69"/>
     </row>
     <row r="33" spans="2:23" ht="29" x14ac:dyDescent="0.35">
       <c r="B33" s="8" t="s">
@@ -2387,7 +2387,7 @@
       </c>
       <c r="H39" s="22">
         <f>SUM(H24:H37)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I39" s="23">
         <f>SUM(I24:I37)</f>
@@ -2395,7 +2395,7 @@
       </c>
       <c r="J39" s="24">
         <f>SUM(J24:J37)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2404,7 +2404,7 @@
       </c>
       <c r="H40" s="25">
         <f>SUM(H25:H36)/ROWS(H25:H36)*100</f>
-        <v>58.333333333333336</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="I40" s="26">
         <f>SUM(I25:I36)/ROWS(I25:I36)*100</f>
@@ -2412,22 +2412,22 @@
       </c>
       <c r="J40" s="27">
         <f>SUM(J25:J36)/ROWS(J25:J36)*100</f>
-        <v>41.666666666666671</v>
+        <v>33.333333333333329</v>
       </c>
     </row>
     <row r="43" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="44" spans="2:23" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B44" s="61" t="s">
+      <c r="B44" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="C44" s="62"/>
-      <c r="D44" s="62"/>
-      <c r="E44" s="62"/>
-      <c r="F44" s="62"/>
-      <c r="G44" s="62"/>
-      <c r="H44" s="62"/>
-      <c r="I44" s="62"/>
-      <c r="J44" s="63"/>
+      <c r="C44" s="47"/>
+      <c r="D44" s="47"/>
+      <c r="E44" s="47"/>
+      <c r="F44" s="47"/>
+      <c r="G44" s="47"/>
+      <c r="H44" s="47"/>
+      <c r="I44" s="47"/>
+      <c r="J44" s="48"/>
       <c r="M44" s="33" t="s">
         <v>27</v>
       </c>
@@ -2435,49 +2435,49 @@
         <v>28</v>
       </c>
       <c r="O44" s="34"/>
-      <c r="P44" s="58" t="s">
+      <c r="P44" s="70" t="s">
         <v>46</v>
       </c>
-      <c r="Q44" s="58"/>
-      <c r="R44" s="58"/>
-      <c r="S44" s="58"/>
-      <c r="T44" s="58"/>
-      <c r="U44" s="58"/>
-      <c r="V44" s="58"/>
-      <c r="W44" s="59"/>
+      <c r="Q44" s="70"/>
+      <c r="R44" s="70"/>
+      <c r="S44" s="70"/>
+      <c r="T44" s="70"/>
+      <c r="U44" s="70"/>
+      <c r="V44" s="70"/>
+      <c r="W44" s="71"/>
     </row>
     <row r="45" spans="2:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B45" s="64" t="s">
+      <c r="B45" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="C45" s="66" t="s">
+      <c r="C45" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="D45" s="66" t="s">
+      <c r="D45" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="E45" s="66" t="s">
+      <c r="E45" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="F45" s="66" t="s">
+      <c r="F45" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="G45" s="68" t="s">
+      <c r="G45" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="H45" s="70" t="s">
+      <c r="H45" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="I45" s="71"/>
-      <c r="J45" s="72"/>
+      <c r="I45" s="56"/>
+      <c r="J45" s="57"/>
     </row>
     <row r="46" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B46" s="65"/>
-      <c r="C46" s="67"/>
-      <c r="D46" s="67"/>
-      <c r="E46" s="67"/>
-      <c r="F46" s="67"/>
-      <c r="G46" s="69"/>
+      <c r="B46" s="50"/>
+      <c r="C46" s="52"/>
+      <c r="D46" s="52"/>
+      <c r="E46" s="52"/>
+      <c r="F46" s="52"/>
+      <c r="G46" s="54"/>
       <c r="H46" s="14" t="s">
         <v>14</v>
       </c>
@@ -2487,19 +2487,19 @@
       <c r="J46" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="M46" s="49" t="s">
+      <c r="M46" s="61" t="s">
         <v>69</v>
       </c>
-      <c r="N46" s="50"/>
-      <c r="O46" s="50"/>
-      <c r="P46" s="50"/>
-      <c r="Q46" s="50"/>
-      <c r="R46" s="50"/>
-      <c r="S46" s="50"/>
-      <c r="T46" s="50"/>
-      <c r="U46" s="50"/>
-      <c r="V46" s="50"/>
-      <c r="W46" s="51"/>
+      <c r="N46" s="62"/>
+      <c r="O46" s="62"/>
+      <c r="P46" s="62"/>
+      <c r="Q46" s="62"/>
+      <c r="R46" s="62"/>
+      <c r="S46" s="62"/>
+      <c r="T46" s="62"/>
+      <c r="U46" s="62"/>
+      <c r="V46" s="62"/>
+      <c r="W46" s="63"/>
     </row>
     <row r="47" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B47" s="11"/>
@@ -2511,17 +2511,17 @@
       <c r="H47" s="15"/>
       <c r="I47" s="9"/>
       <c r="J47" s="10"/>
-      <c r="M47" s="52"/>
-      <c r="N47" s="53"/>
-      <c r="O47" s="53"/>
-      <c r="P47" s="53"/>
-      <c r="Q47" s="53"/>
-      <c r="R47" s="53"/>
-      <c r="S47" s="53"/>
-      <c r="T47" s="53"/>
-      <c r="U47" s="53"/>
-      <c r="V47" s="53"/>
-      <c r="W47" s="54"/>
+      <c r="M47" s="64"/>
+      <c r="N47" s="65"/>
+      <c r="O47" s="65"/>
+      <c r="P47" s="65"/>
+      <c r="Q47" s="65"/>
+      <c r="R47" s="65"/>
+      <c r="S47" s="65"/>
+      <c r="T47" s="65"/>
+      <c r="U47" s="65"/>
+      <c r="V47" s="65"/>
+      <c r="W47" s="66"/>
     </row>
     <row r="48" spans="2:23" ht="29" x14ac:dyDescent="0.35">
       <c r="B48" s="8" t="s">
@@ -2541,17 +2541,17 @@
       </c>
       <c r="I48" s="17"/>
       <c r="J48" s="18"/>
-      <c r="M48" s="52"/>
-      <c r="N48" s="53"/>
-      <c r="O48" s="53"/>
-      <c r="P48" s="53"/>
-      <c r="Q48" s="53"/>
-      <c r="R48" s="53"/>
-      <c r="S48" s="53"/>
-      <c r="T48" s="53"/>
-      <c r="U48" s="53"/>
-      <c r="V48" s="53"/>
-      <c r="W48" s="54"/>
+      <c r="M48" s="64"/>
+      <c r="N48" s="65"/>
+      <c r="O48" s="65"/>
+      <c r="P48" s="65"/>
+      <c r="Q48" s="65"/>
+      <c r="R48" s="65"/>
+      <c r="S48" s="65"/>
+      <c r="T48" s="65"/>
+      <c r="U48" s="65"/>
+      <c r="V48" s="65"/>
+      <c r="W48" s="66"/>
     </row>
     <row r="49" spans="2:23" ht="29" x14ac:dyDescent="0.35">
       <c r="B49" s="8" t="s">
@@ -2571,17 +2571,17 @@
       </c>
       <c r="I49" s="17"/>
       <c r="J49" s="18"/>
-      <c r="M49" s="52"/>
-      <c r="N49" s="53"/>
-      <c r="O49" s="53"/>
-      <c r="P49" s="53"/>
-      <c r="Q49" s="53"/>
-      <c r="R49" s="53"/>
-      <c r="S49" s="53"/>
-      <c r="T49" s="53"/>
-      <c r="U49" s="53"/>
-      <c r="V49" s="53"/>
-      <c r="W49" s="54"/>
+      <c r="M49" s="64"/>
+      <c r="N49" s="65"/>
+      <c r="O49" s="65"/>
+      <c r="P49" s="65"/>
+      <c r="Q49" s="65"/>
+      <c r="R49" s="65"/>
+      <c r="S49" s="65"/>
+      <c r="T49" s="65"/>
+      <c r="U49" s="65"/>
+      <c r="V49" s="65"/>
+      <c r="W49" s="66"/>
     </row>
     <row r="50" spans="2:23" ht="29" x14ac:dyDescent="0.35">
       <c r="B50" s="8" t="s">
@@ -2603,17 +2603,17 @@
         <v>1</v>
       </c>
       <c r="J50" s="18"/>
-      <c r="M50" s="52"/>
-      <c r="N50" s="53"/>
-      <c r="O50" s="53"/>
-      <c r="P50" s="53"/>
-      <c r="Q50" s="53"/>
-      <c r="R50" s="53"/>
-      <c r="S50" s="53"/>
-      <c r="T50" s="53"/>
-      <c r="U50" s="53"/>
-      <c r="V50" s="53"/>
-      <c r="W50" s="54"/>
+      <c r="M50" s="64"/>
+      <c r="N50" s="65"/>
+      <c r="O50" s="65"/>
+      <c r="P50" s="65"/>
+      <c r="Q50" s="65"/>
+      <c r="R50" s="65"/>
+      <c r="S50" s="65"/>
+      <c r="T50" s="65"/>
+      <c r="U50" s="65"/>
+      <c r="V50" s="65"/>
+      <c r="W50" s="66"/>
     </row>
     <row r="51" spans="2:23" ht="29" x14ac:dyDescent="0.35">
       <c r="B51" s="8" t="s">
@@ -2633,17 +2633,17 @@
       </c>
       <c r="I51" s="17"/>
       <c r="J51" s="18"/>
-      <c r="M51" s="52"/>
-      <c r="N51" s="53"/>
-      <c r="O51" s="53"/>
-      <c r="P51" s="53"/>
-      <c r="Q51" s="53"/>
-      <c r="R51" s="53"/>
-      <c r="S51" s="53"/>
-      <c r="T51" s="53"/>
-      <c r="U51" s="53"/>
-      <c r="V51" s="53"/>
-      <c r="W51" s="54"/>
+      <c r="M51" s="64"/>
+      <c r="N51" s="65"/>
+      <c r="O51" s="65"/>
+      <c r="P51" s="65"/>
+      <c r="Q51" s="65"/>
+      <c r="R51" s="65"/>
+      <c r="S51" s="65"/>
+      <c r="T51" s="65"/>
+      <c r="U51" s="65"/>
+      <c r="V51" s="65"/>
+      <c r="W51" s="66"/>
     </row>
     <row r="52" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B52" s="4"/>
@@ -2655,30 +2655,30 @@
       <c r="H52" s="19"/>
       <c r="I52" s="20"/>
       <c r="J52" s="21"/>
-      <c r="M52" s="52"/>
-      <c r="N52" s="53"/>
-      <c r="O52" s="53"/>
-      <c r="P52" s="53"/>
-      <c r="Q52" s="53"/>
-      <c r="R52" s="53"/>
-      <c r="S52" s="53"/>
-      <c r="T52" s="53"/>
-      <c r="U52" s="53"/>
-      <c r="V52" s="53"/>
-      <c r="W52" s="54"/>
+      <c r="M52" s="64"/>
+      <c r="N52" s="65"/>
+      <c r="O52" s="65"/>
+      <c r="P52" s="65"/>
+      <c r="Q52" s="65"/>
+      <c r="R52" s="65"/>
+      <c r="S52" s="65"/>
+      <c r="T52" s="65"/>
+      <c r="U52" s="65"/>
+      <c r="V52" s="65"/>
+      <c r="W52" s="66"/>
     </row>
     <row r="53" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="M53" s="52"/>
-      <c r="N53" s="53"/>
-      <c r="O53" s="53"/>
-      <c r="P53" s="53"/>
-      <c r="Q53" s="53"/>
-      <c r="R53" s="53"/>
-      <c r="S53" s="53"/>
-      <c r="T53" s="53"/>
-      <c r="U53" s="53"/>
-      <c r="V53" s="53"/>
-      <c r="W53" s="54"/>
+      <c r="M53" s="64"/>
+      <c r="N53" s="65"/>
+      <c r="O53" s="65"/>
+      <c r="P53" s="65"/>
+      <c r="Q53" s="65"/>
+      <c r="R53" s="65"/>
+      <c r="S53" s="65"/>
+      <c r="T53" s="65"/>
+      <c r="U53" s="65"/>
+      <c r="V53" s="65"/>
+      <c r="W53" s="66"/>
     </row>
     <row r="54" spans="2:23" x14ac:dyDescent="0.35">
       <c r="G54" s="30" t="s">
@@ -2696,17 +2696,17 @@
         <f>SUM(J47:J52)</f>
         <v>0</v>
       </c>
-      <c r="M54" s="52"/>
-      <c r="N54" s="53"/>
-      <c r="O54" s="53"/>
-      <c r="P54" s="53"/>
-      <c r="Q54" s="53"/>
-      <c r="R54" s="53"/>
-      <c r="S54" s="53"/>
-      <c r="T54" s="53"/>
-      <c r="U54" s="53"/>
-      <c r="V54" s="53"/>
-      <c r="W54" s="54"/>
+      <c r="M54" s="64"/>
+      <c r="N54" s="65"/>
+      <c r="O54" s="65"/>
+      <c r="P54" s="65"/>
+      <c r="Q54" s="65"/>
+      <c r="R54" s="65"/>
+      <c r="S54" s="65"/>
+      <c r="T54" s="65"/>
+      <c r="U54" s="65"/>
+      <c r="V54" s="65"/>
+      <c r="W54" s="66"/>
     </row>
     <row r="55" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G55" s="31" t="s">
@@ -2724,35 +2724,35 @@
         <f>SUM(J48:J51)/ROWS(J48:J51)*100</f>
         <v>0</v>
       </c>
-      <c r="M55" s="55"/>
-      <c r="N55" s="56"/>
-      <c r="O55" s="56"/>
-      <c r="P55" s="56"/>
-      <c r="Q55" s="56"/>
-      <c r="R55" s="56"/>
-      <c r="S55" s="56"/>
-      <c r="T55" s="56"/>
-      <c r="U55" s="56"/>
-      <c r="V55" s="56"/>
-      <c r="W55" s="57"/>
+      <c r="M55" s="67"/>
+      <c r="N55" s="68"/>
+      <c r="O55" s="68"/>
+      <c r="P55" s="68"/>
+      <c r="Q55" s="68"/>
+      <c r="R55" s="68"/>
+      <c r="S55" s="68"/>
+      <c r="T55" s="68"/>
+      <c r="U55" s="68"/>
+      <c r="V55" s="68"/>
+      <c r="W55" s="69"/>
     </row>
     <row r="59" spans="2:23" x14ac:dyDescent="0.35">
-      <c r="O59" s="60" t="s">
+      <c r="O59" s="72" t="s">
         <v>73</v>
       </c>
-      <c r="P59" s="60"/>
-      <c r="Q59" s="60"/>
-      <c r="R59" s="60"/>
-      <c r="S59" s="60"/>
+      <c r="P59" s="72"/>
+      <c r="Q59" s="72"/>
+      <c r="R59" s="72"/>
+      <c r="S59" s="72"/>
     </row>
     <row r="60" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="61" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G61" s="46" t="s">
+      <c r="G61" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="H61" s="47"/>
-      <c r="I61" s="47"/>
-      <c r="J61" s="48"/>
+      <c r="H61" s="59"/>
+      <c r="I61" s="59"/>
+      <c r="J61" s="60"/>
     </row>
     <row r="62" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G62" s="31" t="s">
@@ -2760,39 +2760,23 @@
       </c>
       <c r="H62" s="25">
         <f>SUM(H17+H40+H55)/3</f>
-        <v>56.94444444444445</v>
+        <v>63.888888888888886</v>
       </c>
       <c r="I62" s="26">
         <f>SUM(I17+I40+I55)/3</f>
-        <v>20.833333333333332</v>
+        <v>16.666666666666668</v>
       </c>
       <c r="J62" s="27">
         <f>SUM(J17+J40+J55)/3</f>
-        <v>22.222222222222225</v>
+        <v>19.444444444444443</v>
       </c>
       <c r="K62" s="36">
         <f>SUM(H62:J62)</f>
-        <v>100.00000000000001</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="B21:J21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="H22:J22"/>
     <mergeCell ref="G61:J61"/>
     <mergeCell ref="M4:W13"/>
     <mergeCell ref="P2:W2"/>
@@ -2809,6 +2793,22 @@
     <mergeCell ref="F45:F46"/>
     <mergeCell ref="G45:G46"/>
     <mergeCell ref="H45:J45"/>
+    <mergeCell ref="B21:J21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="H22:J22"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:J3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>